<commit_message>
Update to FU logic: new SQL
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA920AB-AA54-418F-ABAD-89D7B071153B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795DC8A6-D74A-4C26-A167-6759386709F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="451">
   <si>
     <t>setting_name</t>
   </si>
@@ -1359,6 +1359,33 @@
   </si>
   <si>
     <t>Kelbit</t>
+  </si>
+  <si>
+    <t>HHOID</t>
+  </si>
+  <si>
+    <t>BAIRRO</t>
+  </si>
+  <si>
+    <t>for logic</t>
+  </si>
+  <si>
+    <t>HOUSEGRP</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>FNO</t>
+  </si>
+  <si>
+    <t>fno id</t>
+  </si>
+  <si>
+    <t>POID</t>
+  </si>
+  <si>
+    <t>IDOID</t>
   </si>
 </sst>
 </file>
@@ -3904,7 +3931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
@@ -5392,11 +5419,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5435,6 +5462,7 @@
       <c r="D2" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -5446,6 +5474,10 @@
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5457,6 +5489,10 @@
       <c r="C4" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -5580,6 +5616,7 @@
       <c r="D13" s="3" t="s">
         <v>128</v>
       </c>
+      <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -6067,7 +6104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>393</v>
       </c>
@@ -6078,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>400</v>
       </c>
@@ -6089,7 +6126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>404</v>
       </c>
@@ -6100,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>405</v>
       </c>
@@ -6111,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>406</v>
       </c>
@@ -6122,7 +6159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>407</v>
       </c>
@@ -6133,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
         <v>408</v>
       </c>
@@ -6143,6 +6180,97 @@
       <c r="C72" s="3" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>442</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>443</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>445</v>
+      </c>
+      <c r="B76" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>446</v>
+      </c>
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>447</v>
+      </c>
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>449</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>450</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:C28">

</xml_diff>

<commit_message>
upadte to counting and added fuction to add persons when including
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77AE6F7-1FA2-4096-A185-CFA20340987E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24208260-A8C4-4ED2-A5AD-7A8111214A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="479">
   <si>
     <t>setting_name</t>
   </si>
@@ -1455,6 +1455,21 @@
   </si>
   <si>
     <t>Recusou-se a participar do estudo</t>
+  </si>
+  <si>
+    <t>Occasionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("CONS") != "2" </t>
+  </si>
+  <si>
+    <t>Nem sempre</t>
+  </si>
+  <si>
+    <t>Cirúrgia / Pano</t>
+  </si>
+  <si>
+    <t>Surgery / Cloth</t>
   </si>
 </sst>
 </file>
@@ -2010,11 +2025,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:P222"/>
+  <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4041,147 +4056,150 @@
       <c r="G181" s="29"/>
     </row>
     <row r="182" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>317</v>
-      </c>
       <c r="B182" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="C182" t="s">
+        <v>475</v>
       </c>
       <c r="D182" s="3"/>
       <c r="G182" s="29"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D183" s="18" t="s">
+    <row r="183" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>317</v>
+      </c>
+      <c r="B183" t="s">
+        <v>52</v>
+      </c>
+      <c r="D183" s="3"/>
+      <c r="G183" s="29"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D184" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G183" s="27" t="s">
+      <c r="G184" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H183" s="16" t="s">
+      <c r="H184" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="184" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D184" s="3" t="s">
+    <row r="185" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D185" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G184" s="29" t="s">
+      <c r="G185" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H184" t="s">
+      <c r="H185" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D185" s="18" t="s">
+    <row r="186" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D186" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E185" s="16" t="s">
+      <c r="E186" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F185" s="16" t="s">
+      <c r="F186" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="G185" s="27" t="s">
+      <c r="G186" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="H185" s="18" t="s">
+      <c r="H186" s="18" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="16" t="s">
+    <row r="187" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C186" s="16" t="s">
+      <c r="C187" s="16" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D187" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F187" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="G187" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="H187" s="16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D188" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F188" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="G188" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H188" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D189" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E189" t="s">
         <v>48</v>
       </c>
-      <c r="F188" s="27" t="s">
+      <c r="F189" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="G188" s="16"/>
-    </row>
-    <row r="189" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="16" t="s">
+      <c r="G189" s="16"/>
+    </row>
+    <row r="190" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B190" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C189" s="16" t="s">
+      <c r="C190" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="F189" s="27"/>
-      <c r="G189" s="16"/>
-    </row>
-    <row r="190" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D190" s="18" t="s">
+      <c r="F190" s="27"/>
+      <c r="G190" s="16"/>
+    </row>
+    <row r="191" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D191" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F190" s="27" t="s">
+      <c r="F191" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="G190" s="16"/>
-      <c r="I190" s="16" t="s">
+      <c r="G191" s="16"/>
+      <c r="I191" s="16" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F191" s="27"/>
-      <c r="G191" s="16"/>
     </row>
     <row r="192" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C192" s="16" t="s">
-        <v>384</v>
+        <v>39</v>
       </c>
       <c r="F192" s="27"/>
       <c r="G192" s="16"/>
     </row>
     <row r="193" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D193" s="18" t="s">
+      <c r="B193" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C193" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="F193" s="27"/>
+      <c r="G193" s="16"/>
+    </row>
+    <row r="194" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D194" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F193" s="27" t="s">
+      <c r="F194" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="G193" s="16" t="s">
+      <c r="G194" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="H193" s="16" t="s">
+      <c r="H194" s="16" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="194" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F194" s="27"/>
-      <c r="G194" s="16"/>
     </row>
     <row r="195" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="16" t="s">
@@ -4192,150 +4210,152 @@
     </row>
     <row r="196" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F196" s="27"/>
       <c r="G196" s="16"/>
     </row>
     <row r="197" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C197" s="16" t="s">
-        <v>318</v>
+        <v>53</v>
       </c>
       <c r="F197" s="27"/>
       <c r="G197" s="16"/>
     </row>
     <row r="198" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" t="s">
-        <v>52</v>
+      <c r="B198" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C198" s="16" t="s">
+        <v>318</v>
       </c>
       <c r="F198" s="27"/>
       <c r="G198" s="16"/>
     </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D199" s="18" t="s">
+    <row r="199" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>52</v>
+      </c>
+      <c r="F199" s="27"/>
+      <c r="G199" s="16"/>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D200" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G199" s="27" t="s">
+      <c r="G200" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H199" s="16" t="s">
+      <c r="H200" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="200" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D200" s="3" t="s">
+    <row r="201" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D201" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E200" s="16" t="s">
+      <c r="E201" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F200" s="16" t="s">
+      <c r="F201" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="G200" s="27" t="s">
+      <c r="G201" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H200" s="16" t="s">
+      <c r="H201" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="201" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="16" t="s">
+    <row r="202" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D201" s="3"/>
-    </row>
-    <row r="202" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>52</v>
       </c>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D203" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G203" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H203" s="16" t="s">
-        <v>134</v>
-      </c>
+      <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D204" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F204" s="16" t="s">
-        <v>321</v>
+        <v>40</v>
       </c>
       <c r="G204" s="27" t="s">
-        <v>403</v>
+        <v>133</v>
       </c>
       <c r="H204" s="16" t="s">
-        <v>404</v>
+        <v>134</v>
       </c>
     </row>
     <row r="205" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D205" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F205" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G205" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="H205" s="16" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D206" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E205" s="16" t="s">
+      <c r="E206" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F205" s="16" t="s">
+      <c r="F206" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="G205" s="27" t="s">
+      <c r="G206" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H205" s="16" t="s">
+      <c r="H206" s="16" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B206" s="16" t="s">
+    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B207" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C206" s="16" t="s">
+      <c r="C207" s="16" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D207" s="18" t="s">
+    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D208" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F207" s="16" t="s">
+      <c r="F208" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="G207" s="29" t="s">
+      <c r="G208" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="H207" t="s">
+      <c r="H208" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B208" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="209" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B209" s="16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="210" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B210" s="16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="211" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B211" s="16" t="s">
-        <v>421</v>
+        <v>39</v>
       </c>
     </row>
     <row r="212" spans="2:16" x14ac:dyDescent="0.25">
@@ -4345,107 +4365,117 @@
     </row>
     <row r="213" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B213" s="16" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="214" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B214" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="215" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B215" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C213" s="16" t="s">
+      <c r="C215" s="16" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="214" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
+    <row r="216" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
         <v>52</v>
       </c>
-      <c r="D214" s="18"/>
-      <c r="E214" s="16"/>
-      <c r="F214" s="16"/>
-      <c r="G214" s="27"/>
-      <c r="H214" s="16"/>
-    </row>
-    <row r="215" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D215" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G215" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H215" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="216" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D216" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D216" s="18"/>
       <c r="E216" s="16"/>
       <c r="F216" s="16"/>
-      <c r="G216" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="H216" s="16" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="217" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G216" s="27"/>
+      <c r="H216" s="16"/>
+    </row>
+    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D217" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E217" s="16"/>
-      <c r="F217" s="16"/>
       <c r="G217" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H217" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D218" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E218" s="16"/>
+      <c r="F218" s="16"/>
+      <c r="G218" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="H218" s="16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="219" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D219" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E219" s="16"/>
+      <c r="F219" s="16"/>
+      <c r="G219" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="H217" s="16" t="s">
+      <c r="H219" s="16" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D218" t="s">
+    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D220" t="s">
         <v>73</v>
       </c>
-      <c r="F218" t="s">
+      <c r="F220" t="s">
         <v>240</v>
       </c>
-      <c r="G218" t="s">
+      <c r="G220" t="s">
         <v>405</v>
       </c>
-      <c r="H218" t="s">
+      <c r="H220" t="s">
         <v>406</v>
       </c>
-      <c r="O218" s="16"/>
-      <c r="P218" t="s">
+      <c r="O220" s="16"/>
+      <c r="P220" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="219" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D219" t="s">
+    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D221" t="s">
         <v>73</v>
       </c>
-      <c r="F219" t="s">
+      <c r="F221" t="s">
         <v>241</v>
       </c>
-      <c r="G219" t="s">
+      <c r="G221" t="s">
         <v>408</v>
       </c>
-      <c r="H219" t="s">
+      <c r="H221" t="s">
         <v>409</v>
       </c>
-      <c r="O219" s="16"/>
-      <c r="P219" t="s">
+      <c r="O221" s="16"/>
+      <c r="P221" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
+    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="221" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B221" s="16" t="s">
+    <row r="223" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B223" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B222" s="16" t="s">
+    <row r="224" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B224" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4514,11 +4544,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5907,37 +5937,37 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="7"/>
-      <c r="C104" s="23"/>
+      <c r="A104" t="s">
+        <v>214</v>
+      </c>
+      <c r="B104" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C104" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>218</v>
-      </c>
-      <c r="B105" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C105" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="B105" s="7"/>
+      <c r="C105" s="23"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>218</v>
       </c>
       <c r="B106" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C106" s="24" t="s">
-        <v>219</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C106" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,21 +5975,45 @@
         <v>218</v>
       </c>
       <c r="B107" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C107" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>218</v>
+      </c>
+      <c r="B108" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="7"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="7"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="7"/>
@@ -6008,6 +6062,9 @@
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="7"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Fixed HOSPDIA: should not be session variable
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92654738-13E7-4665-8D0C-5F838EC9A96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C645724E-8C6E-4993-B735-5D645AF3DB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -2028,8 +2028,8 @@
   <dimension ref="A1:P224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4491,7 +4491,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,7 +4546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
@@ -6143,9 +6143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6822,7 +6822,7 @@
         <v>74</v>
       </c>
       <c r="C65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -6833,7 +6833,7 @@
         <v>76</v>
       </c>
       <c r="C66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed questions on events
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92654738-13E7-4665-8D0C-5F838EC9A96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F229EE0C-2955-46B0-A725-D26B9579DC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="480">
   <si>
     <t>setting_name</t>
   </si>
@@ -1470,6 +1470,9 @@
   </si>
   <si>
     <t>Surgery / Cloth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("EVENT") === "OLD QUESTION REMOVED 021120" </t>
   </si>
 </sst>
 </file>
@@ -2025,11 +2028,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:P224"/>
+  <dimension ref="A1:P226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,64 +2872,45 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="20"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G72" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>332</v>
-      </c>
+      <c r="F73" s="20"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D74" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F74" s="16" t="s">
-        <v>294</v>
+        <v>40</v>
       </c>
       <c r="G74" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="H74" s="18" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D75" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="F75" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="G75" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="H75" s="18" t="s">
-        <v>274</v>
+        <v>40</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
@@ -2934,130 +2918,139 @@
         <v>37</v>
       </c>
       <c r="E76" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D78" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="F76" s="16" t="s">
+      <c r="F78" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="G76" s="27" t="s">
+      <c r="G78" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="H76" s="18" t="s">
+      <c r="H78" s="18" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G80" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D81" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G81" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H81" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D82" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G83" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H83" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D84" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E84" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F82" s="16" t="s">
+      <c r="F84" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="G82" s="27" t="s">
+      <c r="G84" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="H82" s="18" t="s">
+      <c r="H84" s="18" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="16" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B86" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G85" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H85" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G86" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H86" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D87" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F87" s="16" t="s">
-        <v>280</v>
+        <v>40</v>
       </c>
       <c r="G87" s="27" t="s">
-        <v>453</v>
-      </c>
-      <c r="H87" s="18" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>282</v>
+        <v>133</v>
+      </c>
+      <c r="H87" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H88" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3065,16 +3058,16 @@
         <v>37</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>210</v>
+        <v>59</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G89" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="H89" s="16" t="s">
-        <v>211</v>
+        <v>453</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3082,7 +3075,7 @@
         <v>38</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3090,21 +3083,24 @@
         <v>37</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F91" s="16" t="s">
-        <v>365</v>
+        <v>281</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>278</v>
+        <v>212</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>279</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,16 +3108,16 @@
         <v>37</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F93" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G93" s="27" t="s">
-        <v>65</v>
+        <v>278</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>66</v>
+        <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3130,122 +3126,122 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C95" s="16" t="s">
-        <v>284</v>
+      <c r="D95" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="G95" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H95" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F96" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="G96" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="H96" s="16" t="s">
-        <v>286</v>
+      <c r="B96" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B97" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D98" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="G98" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B98" s="16" t="s">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B101" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D100" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G100" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H100" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D101" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G101" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H101" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D102" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G102" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G103" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H103" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D104" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E104" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F102" s="16" t="s">
+      <c r="F104" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="G102" s="27" t="s">
+      <c r="G104" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="H102" s="16" t="s">
+      <c r="H104" s="16" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B103" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B104" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B105" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D106" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G106" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H106" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D107" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G107" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="H107" s="16" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -3253,50 +3249,32 @@
         <v>40</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>433</v>
+        <v>133</v>
       </c>
       <c r="H108" s="16" t="s">
-        <v>448</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D109" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F109" s="16" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>434</v>
+        <v>141</v>
       </c>
       <c r="H109" s="16" t="s">
-        <v>435</v>
-      </c>
-      <c r="K109" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="L109" s="16" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D110" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F110" s="16" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H110" s="16" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,13 +3285,19 @@
         <v>59</v>
       </c>
       <c r="F111" s="16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>439</v>
+        <v>435</v>
+      </c>
+      <c r="K111" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="L111" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -3324,99 +3308,99 @@
         <v>59</v>
       </c>
       <c r="F112" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G112" s="27" t="s">
+        <v>436</v>
+      </c>
+      <c r="H112" s="16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D113" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G113" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D114" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F114" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G112" s="27" t="s">
+      <c r="G114" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="H112" s="16" t="s">
+      <c r="H114" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="K112" s="16" t="s">
+      <c r="K114" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L112" s="16" t="s">
+      <c r="L114" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="16" t="s">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="16" t="s">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D115" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G115" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H115" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D116" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G116" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D117" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G117" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H117" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D118" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G118" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H118" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D119" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G119" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="H117" s="16" t="s">
+      <c r="H119" s="16" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D118" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E118" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F118" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G118" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="H118" s="16" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D119" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E119" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F119" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="G119" s="27" t="s">
-        <v>444</v>
-      </c>
-      <c r="H119" s="16" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D120" s="18" t="s">
         <v>37</v>
       </c>
@@ -3424,429 +3408,453 @@
         <v>59</v>
       </c>
       <c r="F120" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G120" s="27" t="s">
+        <v>442</v>
+      </c>
+      <c r="H120" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D121" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F121" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="G121" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="H121" s="16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D122" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F122" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="G120" s="27" t="s">
+      <c r="G122" s="27" t="s">
         <v>446</v>
       </c>
-      <c r="H120" s="16" t="s">
+      <c r="H122" s="16" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="16" t="s">
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="16" t="s">
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D123" s="18" t="s">
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D125" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G123" s="27" t="s">
+      <c r="G125" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H123" s="16" t="s">
+      <c r="H125" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D124" s="18" t="s">
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D126" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G124" s="27" t="s">
+      <c r="G126" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="H124" s="16" t="s">
+      <c r="H126" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D125" s="18" t="s">
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D127" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E125" s="16" t="s">
+      <c r="E127" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F125" s="16" t="s">
+      <c r="F127" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="G125" s="27" t="s">
+      <c r="G127" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="H125" s="16" t="s">
+      <c r="H127" s="16" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="16" t="s">
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C126" s="16" t="s">
+      <c r="C128" s="16" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D127" s="18" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D129" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F127" s="16" t="s">
+      <c r="F129" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G127" s="27" t="s">
+      <c r="G129" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="H127" s="16" t="s">
+      <c r="H129" s="16" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D128" s="18" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D130" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="E130" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F128" s="16" t="s">
+      <c r="F130" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G128" s="27" t="s">
+      <c r="G130" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="H128" s="16" t="s">
+      <c r="H130" s="16" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B129" s="16" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B130" s="16" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C132" s="16" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D131" s="18" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D133" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F131" s="16" t="s">
+      <c r="F133" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="G131" s="27" t="s">
+      <c r="G133" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="H131" s="16" t="s">
+      <c r="H133" s="16" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B133" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B134" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="B135" s="16" t="s">
+      <c r="B137" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D136" s="18" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D138" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G136" s="27" t="s">
+      <c r="G138" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H136" s="16" t="s">
+      <c r="H138" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D137" s="3" t="s">
+    <row r="139" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G137" s="29" t="s">
+      <c r="G139" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H139" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D138" s="18" t="s">
+    <row r="140" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="E140" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F138" s="16" t="s">
+      <c r="F140" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="G138" s="29" t="s">
+      <c r="G140" s="29" t="s">
         <v>457</v>
       </c>
-      <c r="H138" t="s">
+      <c r="H140" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="16" t="s">
+    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C139" s="16" t="s">
+      <c r="C141" s="16" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D140" s="18" t="s">
+    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F140" s="31" t="s">
+      <c r="F142" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="G140" s="27" t="s">
+      <c r="G142" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H140" s="16" t="s">
+      <c r="H142" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D141" s="18" t="s">
+    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E143" t="s">
         <v>48</v>
       </c>
-      <c r="F141" s="27" t="s">
+      <c r="F143" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="G141" s="16"/>
-    </row>
-    <row r="142" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="16" t="s">
+      <c r="G143" s="16"/>
+    </row>
+    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="16" t="s">
+      <c r="C144" s="16" t="s">
         <v>377</v>
-      </c>
-      <c r="F142" s="27"/>
-      <c r="G142" s="16"/>
-    </row>
-    <row r="143" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D143" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F143" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="G143" s="16"/>
-      <c r="I143" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F144" s="27"/>
       <c r="G144" s="16"/>
     </row>
-    <row r="145" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="16" t="s">
+    <row r="145" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F145" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="G145" s="16"/>
+      <c r="I145" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="146" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F146" s="27"/>
+      <c r="G146" s="16"/>
+    </row>
+    <row r="147" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C145" s="16" t="s">
+      <c r="C147" s="16" t="s">
         <v>379</v>
-      </c>
-      <c r="F145" s="27"/>
-      <c r="G145" s="16"/>
-    </row>
-    <row r="146" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D146" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F146" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="G146" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H146" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="147" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F147" s="27"/>
       <c r="G147" s="16"/>
     </row>
-    <row r="148" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="16" t="s">
+    <row r="148" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D148" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F148" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="G148" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H148" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="G148" s="16"/>
-    </row>
-    <row r="149" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F149" s="27"/>
       <c r="G149" s="16"/>
     </row>
-    <row r="150" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="F150" s="27"/>
+        <v>39</v>
+      </c>
       <c r="G150" s="16"/>
     </row>
-    <row r="151" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F151" s="27"/>
       <c r="G151" s="16"/>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D152" s="18" t="s">
+    <row r="152" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F152" s="27"/>
+      <c r="G152" s="16"/>
+    </row>
+    <row r="153" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F153" s="27"/>
+      <c r="G153" s="16"/>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D154" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G152" s="27" t="s">
+      <c r="G154" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H152" s="16" t="s">
+      <c r="H154" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D153" s="3" t="s">
+    <row r="155" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="E155" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F153" s="16" t="s">
+      <c r="F155" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="G153" s="27" t="s">
+      <c r="G155" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H153" s="16" t="s">
+      <c r="H155" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="154" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="16" t="s">
+    <row r="156" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G154" s="16"/>
-    </row>
-    <row r="155" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="16" t="s">
+      <c r="G156" s="16"/>
+    </row>
+    <row r="157" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F155" s="27"/>
-      <c r="G155" s="16"/>
-    </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D156" s="18" t="s">
+      <c r="F157" s="27"/>
+      <c r="G157" s="16"/>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D158" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G156" s="27" t="s">
+      <c r="G158" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H156" s="16" t="s">
+      <c r="H158" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D157" s="18" t="s">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D159" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F157" s="16" t="s">
+      <c r="F159" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="G157" s="27" t="s">
+      <c r="G159" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="H157" s="16" t="s">
+      <c r="H159" s="16" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D158" s="18" t="s">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D160" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="E160" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F158" s="16" t="s">
+      <c r="F160" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="G158" s="27" t="s">
+      <c r="G160" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H158" s="16" t="s">
+      <c r="H160" s="16" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B159" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C159" s="16" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D160" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="G160" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H160" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B161" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B162" s="16" t="s">
-        <v>53</v>
+      <c r="D162" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="G162" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H162" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -3854,117 +3862,100 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B164" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B165" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>78</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>52</v>
       </c>
-      <c r="D164" s="3"/>
-      <c r="G164" s="29"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D165" s="18" t="s">
+      <c r="D166" s="3"/>
+      <c r="G166" s="29"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D167" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G165" s="27" t="s">
+      <c r="G167" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H165" s="16" t="s">
+      <c r="H167" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="166" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D166" s="3" t="s">
+    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D168" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G166" s="29" t="s">
+      <c r="G168" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H166" t="s">
+      <c r="H168" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="167" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D167" s="3" t="s">
+    <row r="169" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D169" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E169" t="s">
         <v>59</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F169" t="s">
         <v>78</v>
       </c>
-      <c r="G167" s="29" t="s">
+      <c r="G169" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H169" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
+    <row r="170" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>53</v>
       </c>
-      <c r="D168" s="3"/>
-      <c r="G168" s="29"/>
-    </row>
-    <row r="169" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
+      <c r="D170" s="3"/>
+      <c r="G170" s="29"/>
+    </row>
+    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
         <v>52</v>
       </c>
-      <c r="D169" s="3"/>
-      <c r="G169" s="29"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D170" s="18" t="s">
+      <c r="D171" s="3"/>
+      <c r="G171" s="29"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D172" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G170" s="27" t="s">
+      <c r="G172" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H170" s="16" t="s">
+      <c r="H172" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D171" s="3" t="s">
+    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D173" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G171" s="29" t="s">
+      <c r="G173" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H171" t="s">
+      <c r="H173" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D172" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E172" t="s">
-        <v>59</v>
-      </c>
-      <c r="F172" t="s">
-        <v>368</v>
-      </c>
-      <c r="G172" s="29" t="s">
-        <v>459</v>
-      </c>
-      <c r="H172" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>38</v>
-      </c>
-      <c r="C173" t="s">
-        <v>399</v>
-      </c>
-      <c r="D173" s="3"/>
-      <c r="G173" s="29"/>
     </row>
     <row r="174" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D174" s="3" t="s">
@@ -3974,13 +3965,13 @@
         <v>59</v>
       </c>
       <c r="F174" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G174" s="29" t="s">
-        <v>311</v>
+        <v>459</v>
       </c>
       <c r="H174" t="s">
-        <v>312</v>
+        <v>460</v>
       </c>
     </row>
     <row r="175" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3988,369 +3979,386 @@
         <v>38</v>
       </c>
       <c r="C175" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D175" s="3"/>
       <c r="G175" s="29"/>
     </row>
     <row r="176" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D176" s="3" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="E176" t="s">
+        <v>59</v>
       </c>
       <c r="F176" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G176" s="29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H176" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C177" t="s">
+        <v>400</v>
       </c>
       <c r="D177" s="3"/>
       <c r="G177" s="29"/>
     </row>
-    <row r="178" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E178" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F178" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G178" s="29" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H178" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>39</v>
       </c>
       <c r="D179" s="3"/>
       <c r="G179" s="29"/>
     </row>
-    <row r="180" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>53</v>
-      </c>
-      <c r="D180" s="3"/>
-      <c r="G180" s="29"/>
-    </row>
-    <row r="181" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D180" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E180" t="s">
+        <v>79</v>
+      </c>
+      <c r="F180" t="s">
+        <v>371</v>
+      </c>
+      <c r="G180" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="H180" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>38</v>
-      </c>
-      <c r="C181" t="s">
-        <v>417</v>
+        <v>39</v>
       </c>
       <c r="D181" s="3"/>
       <c r="G181" s="29"/>
     </row>
-    <row r="182" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>38</v>
-      </c>
-      <c r="C182" t="s">
-        <v>475</v>
+        <v>53</v>
       </c>
       <c r="D182" s="3"/>
       <c r="G182" s="29"/>
     </row>
-    <row r="183" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>317</v>
-      </c>
+    <row r="183" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="C183" t="s">
+        <v>417</v>
       </c>
       <c r="D183" s="3"/>
       <c r="G183" s="29"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D184" s="18" t="s">
+    <row r="184" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>38</v>
+      </c>
+      <c r="C184" t="s">
+        <v>475</v>
+      </c>
+      <c r="D184" s="3"/>
+      <c r="G184" s="29"/>
+    </row>
+    <row r="185" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>317</v>
+      </c>
+      <c r="B185" t="s">
+        <v>52</v>
+      </c>
+      <c r="D185" s="3"/>
+      <c r="G185" s="29"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D186" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G184" s="27" t="s">
+      <c r="G186" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H184" s="16" t="s">
+      <c r="H186" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="185" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D185" s="3" t="s">
+    <row r="187" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D187" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G185" s="29" t="s">
+      <c r="G187" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H185" t="s">
+      <c r="H187" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D186" s="18" t="s">
+    <row r="188" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D188" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E186" s="16" t="s">
+      <c r="E188" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F186" s="16" t="s">
+      <c r="F188" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="G186" s="27" t="s">
+      <c r="G188" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="H186" s="18" t="s">
+      <c r="H188" s="18" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="16" t="s">
+    <row r="189" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C187" s="16" t="s">
+      <c r="C189" s="16" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D188" s="18" t="s">
+    <row r="190" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D190" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F188" s="16" t="s">
+      <c r="F190" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="G188" s="27" t="s">
+      <c r="G190" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H188" s="16" t="s">
+      <c r="H190" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D189" s="18" t="s">
+    <row r="191" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D191" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E191" t="s">
         <v>48</v>
       </c>
-      <c r="F189" s="27" t="s">
+      <c r="F191" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="G189" s="16"/>
-    </row>
-    <row r="190" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="16" t="s">
+      <c r="G191" s="16"/>
+    </row>
+    <row r="192" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C190" s="16" t="s">
+      <c r="C192" s="16" t="s">
         <v>383</v>
-      </c>
-      <c r="F190" s="27"/>
-      <c r="G190" s="16"/>
-    </row>
-    <row r="191" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D191" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F191" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="G191" s="16"/>
-      <c r="I191" s="16" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F192" s="27"/>
       <c r="G192" s="16"/>
     </row>
-    <row r="193" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="16" t="s">
+    <row r="193" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D193" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F193" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="G193" s="16"/>
+      <c r="I193" s="16" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F194" s="27"/>
+      <c r="G194" s="16"/>
+    </row>
+    <row r="195" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C193" s="16" t="s">
+      <c r="C195" s="16" t="s">
         <v>384</v>
-      </c>
-      <c r="F193" s="27"/>
-      <c r="G193" s="16"/>
-    </row>
-    <row r="194" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D194" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F194" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="G194" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H194" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="195" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F195" s="27"/>
       <c r="G195" s="16"/>
     </row>
-    <row r="196" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="16" t="s">
+    <row r="196" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D196" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F196" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="G196" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H196" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="F196" s="27"/>
-      <c r="G196" s="16"/>
-    </row>
-    <row r="197" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F197" s="27"/>
       <c r="G197" s="16"/>
     </row>
-    <row r="198" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C198" s="16" t="s">
-        <v>318</v>
+        <v>39</v>
       </c>
       <c r="F198" s="27"/>
       <c r="G198" s="16"/>
     </row>
-    <row r="199" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>52</v>
+    <row r="199" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B199" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="F199" s="27"/>
       <c r="G199" s="16"/>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D200" s="18" t="s">
+    <row r="200" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C200" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F200" s="27"/>
+      <c r="G200" s="16"/>
+    </row>
+    <row r="201" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>52</v>
+      </c>
+      <c r="F201" s="27"/>
+      <c r="G201" s="16"/>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D202" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G200" s="27" t="s">
+      <c r="G202" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H200" s="16" t="s">
+      <c r="H202" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="201" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D201" s="3" t="s">
+    <row r="203" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D203" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E201" s="16" t="s">
+      <c r="E203" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F201" s="16" t="s">
+      <c r="F203" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="G201" s="27" t="s">
+      <c r="G203" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H201" s="16" t="s">
+      <c r="H203" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="202" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="16" t="s">
+    <row r="204" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>52</v>
       </c>
-      <c r="D203" s="3"/>
-    </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D204" s="18" t="s">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D206" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G204" s="27" t="s">
+      <c r="G206" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H204" s="16" t="s">
+      <c r="H206" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D205" s="18" t="s">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D207" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F205" s="16" t="s">
+      <c r="F207" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="G205" s="27" t="s">
+      <c r="G207" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="H205" s="16" t="s">
+      <c r="H207" s="16" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D206" s="18" t="s">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D208" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E206" s="16" t="s">
+      <c r="E208" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F206" s="16" t="s">
+      <c r="F208" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="G206" s="27" t="s">
+      <c r="G208" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H206" s="16" t="s">
+      <c r="H208" s="16" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B207" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C207" s="16" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D208" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F208" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="G208" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H208" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="209" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B209" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C209" s="16" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="210" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B210" s="16" t="s">
-        <v>53</v>
+      <c r="D210" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F210" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="G210" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H210" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="211" spans="2:16" x14ac:dyDescent="0.25">
@@ -4360,12 +4368,12 @@
     </row>
     <row r="212" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B212" s="16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="213" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B213" s="16" t="s">
-        <v>421</v>
+        <v>39</v>
       </c>
     </row>
     <row r="214" spans="2:16" x14ac:dyDescent="0.25">
@@ -4375,107 +4383,117 @@
     </row>
     <row r="215" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B215" s="16" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="216" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B216" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B217" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C215" s="16" t="s">
+      <c r="C217" s="16" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="216" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
+    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
         <v>52</v>
       </c>
-      <c r="D216" s="18"/>
-      <c r="E216" s="16"/>
-      <c r="F216" s="16"/>
-      <c r="G216" s="27"/>
-      <c r="H216" s="16"/>
-    </row>
-    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D217" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G217" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H217" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D218" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D218" s="18"/>
       <c r="E218" s="16"/>
       <c r="F218" s="16"/>
-      <c r="G218" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="H218" s="16" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="219" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G218" s="27"/>
+      <c r="H218" s="16"/>
+    </row>
+    <row r="219" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D219" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E219" s="16"/>
-      <c r="F219" s="16"/>
       <c r="G219" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H219" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D220" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E220" s="16"/>
+      <c r="F220" s="16"/>
+      <c r="G220" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="H220" s="16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D221" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E221" s="16"/>
+      <c r="F221" s="16"/>
+      <c r="G221" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="H219" s="16" t="s">
+      <c r="H221" s="16" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D220" t="s">
+    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D222" t="s">
         <v>73</v>
       </c>
-      <c r="F220" t="s">
+      <c r="F222" t="s">
         <v>240</v>
       </c>
-      <c r="G220" t="s">
+      <c r="G222" t="s">
         <v>405</v>
       </c>
-      <c r="H220" t="s">
+      <c r="H222" t="s">
         <v>406</v>
       </c>
-      <c r="O220" s="16"/>
-      <c r="P220" t="s">
+      <c r="O222" s="16"/>
+      <c r="P222" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D221" t="s">
+    <row r="223" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D223" t="s">
         <v>73</v>
       </c>
-      <c r="F221" t="s">
+      <c r="F223" t="s">
         <v>241</v>
       </c>
-      <c r="G221" t="s">
+      <c r="G223" t="s">
         <v>408</v>
       </c>
-      <c r="H221" t="s">
+      <c r="H223" t="s">
         <v>409</v>
       </c>
-      <c r="O221" s="16"/>
-      <c r="P221" t="s">
+      <c r="O223" s="16"/>
+      <c r="P223" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B222" t="s">
+    <row r="224" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="223" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B223" s="16" t="s">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="224" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B224" s="16" t="s">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4546,8 +4564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alligned with master for merge
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F229EE0C-2955-46B0-A725-D26B9579DC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788E350D-068A-4B7A-BA6E-E7FE9357E283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1582,7 +1582,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1623,6 +1623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2030,9 +2031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:P226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6161,9 +6162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6190,13 +6191,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -6204,13 +6205,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -6218,13 +6219,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -6232,13 +6233,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3" t="b">
+      <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -6246,13 +6247,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="3" t="b">
+      <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -6260,13 +6261,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>390</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="b">
+      <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -6274,13 +6275,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="b">
+      <c r="C8" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -6288,18 +6289,21 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="b">
+      <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="16"/>
@@ -6307,53 +6311,58 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="b">
+      <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>234</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="3" t="b">
+      <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" t="s">
         <v>372</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="b">
+      <c r="C13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" t="s">
         <v>375</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>242</v>
       </c>
       <c r="B16" t="s">
@@ -6364,7 +6373,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" t="s">
         <v>243</v>
       </c>
       <c r="B17" t="s">
@@ -6375,44 +6384,49 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="b">
+      <c r="C18" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="b">
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" t="s">
         <v>290</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" t="s">
         <v>37</v>
       </c>
       <c r="C22" t="b">
@@ -6420,10 +6434,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" t="s">
         <v>74</v>
       </c>
       <c r="C23" t="b">
@@ -6431,43 +6445,43 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" t="s">
         <v>292</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="3" t="b">
+      <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="3" t="b">
+      <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" t="s">
         <v>294</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="3" t="b">
+      <c r="C26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" t="s">
         <v>364</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="b">
@@ -6475,46 +6489,48 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
       <c r="C28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" t="s">
         <v>280</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="3" t="b">
+      <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" t="s">
         <v>281</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="3" t="b">
+      <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" t="s">
         <v>365</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="3" t="b">
+      <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" t="s">
         <v>366</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32" t="b">
@@ -6522,43 +6538,48 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" t="s">
         <v>367</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" t="s">
         <v>73</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+      <c r="A35" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="3" t="b">
+      <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="3" t="b">
+      <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="b">
@@ -6566,10 +6587,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
       <c r="C38" t="b">
@@ -6577,43 +6598,43 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="3" t="b">
+      <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="3" t="b">
+      <c r="C40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" t="s">
         <v>222</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="b">
+      <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" t="s">
         <v>289</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" t="s">
         <v>37</v>
       </c>
       <c r="C42" t="b">
@@ -6621,10 +6642,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" t="s">
         <v>225</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" t="s">
         <v>37</v>
       </c>
       <c r="C43" t="b">
@@ -6632,46 +6653,48 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" t="s">
         <v>227</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="3" t="b">
+      <c r="C44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="3" t="b">
+      <c r="C45" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="3" t="b">
+      <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" t="s">
         <v>295</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" t="s">
         <v>37</v>
       </c>
       <c r="C48" t="b">
@@ -6679,65 +6702,65 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" t="s">
         <v>297</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="3" t="b">
+      <c r="C49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" t="s">
         <v>376</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="3" t="b">
+      <c r="C50" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" t="s">
         <v>380</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="3" t="b">
+      <c r="C51" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" t="s">
         <v>298</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="3" t="b">
+      <c r="C52" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" t="s">
         <v>299</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="3" t="b">
+      <c r="C53" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" t="s">
         <v>302</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" t="s">
         <v>37</v>
       </c>
       <c r="C54" t="b">
@@ -6745,15 +6768,20 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" t="s">
         <v>304</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" t="s">
         <v>73</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -6762,7 +6790,7 @@
       <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="3" t="b">
+      <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6773,7 +6801,7 @@
       <c r="B58" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="3" t="b">
+      <c r="C58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6806,26 +6834,31 @@
       <c r="B61" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" t="s">
         <v>317</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="3" t="b">
+      <c r="C63" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" t="s">
         <v>319</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" t="s">
         <v>30</v>
       </c>
       <c r="C64" t="b">
@@ -6833,29 +6866,29 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" t="s">
         <v>386</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" t="s">
         <v>74</v>
       </c>
       <c r="C65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
+      <c r="A66" t="s">
         <v>385</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" t="s">
         <v>76</v>
       </c>
       <c r="C66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" t="s">
         <v>320</v>
       </c>
       <c r="B67" t="s">
@@ -6866,37 +6899,42 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="A68" t="s">
         <v>321</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" t="s">
         <v>73</v>
       </c>
-      <c r="C68" s="3" t="b">
+      <c r="C68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="A69" t="s">
         <v>322</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="3" t="b">
+      <c r="C69" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+      <c r="A70" t="s">
         <v>323</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -6990,13 +7028,13 @@
       <c r="D78"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" t="s">
         <v>153</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="3" t="b">
+      <c r="C79" t="b">
         <v>0</v>
       </c>
       <c r="D79" s="3" t="s">
@@ -7004,13 +7042,13 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
+      <c r="A80" t="s">
         <v>238</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="3" t="b">
+      <c r="C80" t="b">
         <v>0</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -7019,13 +7057,13 @@
       <c r="J80"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="A81" t="s">
         <v>239</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" t="s">
         <v>73</v>
       </c>
-      <c r="C81" s="3" t="b">
+      <c r="C81" t="b">
         <v>0</v>
       </c>
       <c r="G81"/>
@@ -7034,13 +7072,13 @@
       <c r="J81"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="3" t="b">
+      <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="G82"/>
@@ -7049,35 +7087,35 @@
       <c r="J82"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" t="s">
         <v>73</v>
       </c>
-      <c r="C83" s="3" t="b">
+      <c r="C83" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+      <c r="A84" t="s">
         <v>395</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="3" t="b">
+      <c r="C84" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
+      <c r="A85" t="s">
         <v>396</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" t="s">
         <v>73</v>
       </c>
-      <c r="C85" s="3" t="b">
+      <c r="C85" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Alligned for merge with update
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C645724E-8C6E-4993-B735-5D645AF3DB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788E350D-068A-4B7A-BA6E-E7FE9357E283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="480">
   <si>
     <t>setting_name</t>
   </si>
@@ -1470,6 +1470,9 @@
   </si>
   <si>
     <t>Surgery / Cloth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("EVENT") === "OLD QUESTION REMOVED 021120" </t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1582,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1620,6 +1623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2025,11 +2029,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:P224"/>
+  <dimension ref="A1:P226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,64 +2873,45 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="20"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G72" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>332</v>
-      </c>
+      <c r="F73" s="20"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D74" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F74" s="16" t="s">
-        <v>294</v>
+        <v>40</v>
       </c>
       <c r="G74" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="H74" s="18" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D75" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="F75" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="G75" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="H75" s="18" t="s">
-        <v>274</v>
+        <v>40</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
@@ -2934,130 +2919,139 @@
         <v>37</v>
       </c>
       <c r="E76" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G76" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D78" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="F76" s="16" t="s">
+      <c r="F78" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="G76" s="27" t="s">
+      <c r="G78" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="H76" s="18" t="s">
+      <c r="H78" s="18" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D80" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G80" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D81" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G81" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H81" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D82" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G83" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H83" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D84" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E84" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F82" s="16" t="s">
+      <c r="F84" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="G82" s="27" t="s">
+      <c r="G84" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="H82" s="18" t="s">
+      <c r="H84" s="18" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="16" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B86" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D85" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G85" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H85" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G86" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H86" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D87" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F87" s="16" t="s">
-        <v>280</v>
+        <v>40</v>
       </c>
       <c r="G87" s="27" t="s">
-        <v>453</v>
-      </c>
-      <c r="H87" s="18" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>282</v>
+        <v>133</v>
+      </c>
+      <c r="H87" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H88" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3065,16 +3059,16 @@
         <v>37</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>210</v>
+        <v>59</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G89" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="H89" s="16" t="s">
-        <v>211</v>
+        <v>453</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3082,7 +3076,7 @@
         <v>38</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3090,21 +3084,24 @@
         <v>37</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F91" s="16" t="s">
-        <v>365</v>
+        <v>281</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>278</v>
+        <v>212</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>279</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,16 +3109,16 @@
         <v>37</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F93" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G93" s="27" t="s">
-        <v>65</v>
+        <v>278</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>66</v>
+        <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3130,122 +3127,122 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C95" s="16" t="s">
-        <v>284</v>
+      <c r="D95" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="G95" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H95" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D96" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F96" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="G96" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="H96" s="16" t="s">
-        <v>286</v>
+      <c r="B96" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B97" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D98" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="G98" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B98" s="16" t="s">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B101" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D100" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G100" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H100" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D101" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G101" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="H101" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D102" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G102" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G103" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H103" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D104" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E104" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F102" s="16" t="s">
+      <c r="F104" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="G102" s="27" t="s">
+      <c r="G104" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="H102" s="16" t="s">
+      <c r="H104" s="16" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B103" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B104" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B105" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D106" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G106" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H106" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D107" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G107" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="H107" s="16" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -3253,50 +3250,32 @@
         <v>40</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>433</v>
+        <v>133</v>
       </c>
       <c r="H108" s="16" t="s">
-        <v>448</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D109" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F109" s="16" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>434</v>
+        <v>141</v>
       </c>
       <c r="H109" s="16" t="s">
-        <v>435</v>
-      </c>
-      <c r="K109" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="L109" s="16" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D110" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F110" s="16" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H110" s="16" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,13 +3286,19 @@
         <v>59</v>
       </c>
       <c r="F111" s="16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>439</v>
+        <v>435</v>
+      </c>
+      <c r="K111" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="L111" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -3324,99 +3309,99 @@
         <v>59</v>
       </c>
       <c r="F112" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G112" s="27" t="s">
+        <v>436</v>
+      </c>
+      <c r="H112" s="16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D113" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G113" s="27" t="s">
+        <v>438</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D114" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F114" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G112" s="27" t="s">
+      <c r="G114" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="H112" s="16" t="s">
+      <c r="H114" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="K112" s="16" t="s">
+      <c r="K114" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L112" s="16" t="s">
+      <c r="L114" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="16" t="s">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="16" t="s">
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D115" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G115" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H115" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D116" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G116" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D117" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G117" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H117" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D118" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G118" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="H118" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D119" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G119" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="H117" s="16" t="s">
+      <c r="H119" s="16" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D118" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E118" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F118" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G118" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="H118" s="16" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D119" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E119" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F119" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="G119" s="27" t="s">
-        <v>444</v>
-      </c>
-      <c r="H119" s="16" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D120" s="18" t="s">
         <v>37</v>
       </c>
@@ -3424,429 +3409,453 @@
         <v>59</v>
       </c>
       <c r="F120" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G120" s="27" t="s">
+        <v>442</v>
+      </c>
+      <c r="H120" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D121" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F121" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="G121" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="H121" s="16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D122" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F122" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="G120" s="27" t="s">
+      <c r="G122" s="27" t="s">
         <v>446</v>
       </c>
-      <c r="H120" s="16" t="s">
+      <c r="H122" s="16" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="16" t="s">
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="16" t="s">
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D123" s="18" t="s">
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D125" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G123" s="27" t="s">
+      <c r="G125" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H123" s="16" t="s">
+      <c r="H125" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D124" s="18" t="s">
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D126" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G124" s="27" t="s">
+      <c r="G126" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="H124" s="16" t="s">
+      <c r="H126" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D125" s="18" t="s">
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D127" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E125" s="16" t="s">
+      <c r="E127" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F125" s="16" t="s">
+      <c r="F127" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="G125" s="27" t="s">
+      <c r="G127" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="H125" s="16" t="s">
+      <c r="H127" s="16" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="16" t="s">
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C126" s="16" t="s">
+      <c r="C128" s="16" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D127" s="18" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D129" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F127" s="16" t="s">
+      <c r="F129" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G127" s="27" t="s">
+      <c r="G129" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="H127" s="16" t="s">
+      <c r="H129" s="16" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D128" s="18" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D130" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="E130" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F128" s="16" t="s">
+      <c r="F130" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="G128" s="27" t="s">
+      <c r="G130" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="H128" s="16" t="s">
+      <c r="H130" s="16" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B129" s="16" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B130" s="16" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C132" s="16" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D131" s="18" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D133" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F131" s="16" t="s">
+      <c r="F133" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="G131" s="27" t="s">
+      <c r="G133" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="H131" s="16" t="s">
+      <c r="H133" s="16" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B133" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B134" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="B135" s="16" t="s">
+      <c r="B137" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D136" s="18" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D138" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G136" s="27" t="s">
+      <c r="G138" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H136" s="16" t="s">
+      <c r="H138" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D137" s="3" t="s">
+    <row r="139" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G137" s="29" t="s">
+      <c r="G139" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H139" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D138" s="18" t="s">
+    <row r="140" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="E140" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F138" s="16" t="s">
+      <c r="F140" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="G138" s="29" t="s">
+      <c r="G140" s="29" t="s">
         <v>457</v>
       </c>
-      <c r="H138" t="s">
+      <c r="H140" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="16" t="s">
+    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C139" s="16" t="s">
+      <c r="C141" s="16" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D140" s="18" t="s">
+    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F140" s="31" t="s">
+      <c r="F142" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="G140" s="27" t="s">
+      <c r="G142" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H140" s="16" t="s">
+      <c r="H142" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D141" s="18" t="s">
+    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E143" t="s">
         <v>48</v>
       </c>
-      <c r="F141" s="27" t="s">
+      <c r="F143" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="G141" s="16"/>
-    </row>
-    <row r="142" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="16" t="s">
+      <c r="G143" s="16"/>
+    </row>
+    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="16" t="s">
+      <c r="C144" s="16" t="s">
         <v>377</v>
-      </c>
-      <c r="F142" s="27"/>
-      <c r="G142" s="16"/>
-    </row>
-    <row r="143" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D143" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F143" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="G143" s="16"/>
-      <c r="I143" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F144" s="27"/>
       <c r="G144" s="16"/>
     </row>
-    <row r="145" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="16" t="s">
+    <row r="145" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F145" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="G145" s="16"/>
+      <c r="I145" s="16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="146" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F146" s="27"/>
+      <c r="G146" s="16"/>
+    </row>
+    <row r="147" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C145" s="16" t="s">
+      <c r="C147" s="16" t="s">
         <v>379</v>
-      </c>
-      <c r="F145" s="27"/>
-      <c r="G145" s="16"/>
-    </row>
-    <row r="146" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D146" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F146" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="G146" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H146" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="147" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F147" s="27"/>
       <c r="G147" s="16"/>
     </row>
-    <row r="148" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="16" t="s">
+    <row r="148" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D148" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F148" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="G148" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H148" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="G148" s="16"/>
-    </row>
-    <row r="149" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F149" s="27"/>
       <c r="G149" s="16"/>
     </row>
-    <row r="150" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="F150" s="27"/>
+        <v>39</v>
+      </c>
       <c r="G150" s="16"/>
     </row>
-    <row r="151" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F151" s="27"/>
       <c r="G151" s="16"/>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D152" s="18" t="s">
+    <row r="152" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F152" s="27"/>
+      <c r="G152" s="16"/>
+    </row>
+    <row r="153" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F153" s="27"/>
+      <c r="G153" s="16"/>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D154" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G152" s="27" t="s">
+      <c r="G154" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H152" s="16" t="s">
+      <c r="H154" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D153" s="3" t="s">
+    <row r="155" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="E155" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F153" s="16" t="s">
+      <c r="F155" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="G153" s="27" t="s">
+      <c r="G155" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H153" s="16" t="s">
+      <c r="H155" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="154" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="16" t="s">
+    <row r="156" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G154" s="16"/>
-    </row>
-    <row r="155" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="16" t="s">
+      <c r="G156" s="16"/>
+    </row>
+    <row r="157" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F155" s="27"/>
-      <c r="G155" s="16"/>
-    </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D156" s="18" t="s">
+      <c r="F157" s="27"/>
+      <c r="G157" s="16"/>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D158" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G156" s="27" t="s">
+      <c r="G158" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H156" s="16" t="s">
+      <c r="H158" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D157" s="18" t="s">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D159" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F157" s="16" t="s">
+      <c r="F159" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="G157" s="27" t="s">
+      <c r="G159" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="H157" s="16" t="s">
+      <c r="H159" s="16" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D158" s="18" t="s">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D160" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="E160" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F158" s="16" t="s">
+      <c r="F160" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="G158" s="27" t="s">
+      <c r="G160" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H158" s="16" t="s">
+      <c r="H160" s="16" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B159" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C159" s="16" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D160" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="G160" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H160" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B161" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C161" s="16" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B162" s="16" t="s">
-        <v>53</v>
+      <c r="D162" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="G162" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H162" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -3854,117 +3863,100 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B164" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B165" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>78</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>52</v>
       </c>
-      <c r="D164" s="3"/>
-      <c r="G164" s="29"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D165" s="18" t="s">
+      <c r="D166" s="3"/>
+      <c r="G166" s="29"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D167" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G165" s="27" t="s">
+      <c r="G167" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H165" s="16" t="s">
+      <c r="H167" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="166" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D166" s="3" t="s">
+    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D168" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G166" s="29" t="s">
+      <c r="G168" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H166" t="s">
+      <c r="H168" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="167" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D167" s="3" t="s">
+    <row r="169" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D169" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E169" t="s">
         <v>59</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F169" t="s">
         <v>78</v>
       </c>
-      <c r="G167" s="29" t="s">
+      <c r="G169" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H169" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
+    <row r="170" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>53</v>
       </c>
-      <c r="D168" s="3"/>
-      <c r="G168" s="29"/>
-    </row>
-    <row r="169" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
+      <c r="D170" s="3"/>
+      <c r="G170" s="29"/>
+    </row>
+    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
         <v>52</v>
       </c>
-      <c r="D169" s="3"/>
-      <c r="G169" s="29"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D170" s="18" t="s">
+      <c r="D171" s="3"/>
+      <c r="G171" s="29"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D172" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G170" s="27" t="s">
+      <c r="G172" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H170" s="16" t="s">
+      <c r="H172" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D171" s="3" t="s">
+    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D173" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G171" s="29" t="s">
+      <c r="G173" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H171" t="s">
+      <c r="H173" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D172" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E172" t="s">
-        <v>59</v>
-      </c>
-      <c r="F172" t="s">
-        <v>368</v>
-      </c>
-      <c r="G172" s="29" t="s">
-        <v>459</v>
-      </c>
-      <c r="H172" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B173" t="s">
-        <v>38</v>
-      </c>
-      <c r="C173" t="s">
-        <v>399</v>
-      </c>
-      <c r="D173" s="3"/>
-      <c r="G173" s="29"/>
     </row>
     <row r="174" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D174" s="3" t="s">
@@ -3974,13 +3966,13 @@
         <v>59</v>
       </c>
       <c r="F174" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G174" s="29" t="s">
-        <v>311</v>
+        <v>459</v>
       </c>
       <c r="H174" t="s">
-        <v>312</v>
+        <v>460</v>
       </c>
     </row>
     <row r="175" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3988,369 +3980,386 @@
         <v>38</v>
       </c>
       <c r="C175" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D175" s="3"/>
       <c r="G175" s="29"/>
     </row>
     <row r="176" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D176" s="3" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="E176" t="s">
+        <v>59</v>
       </c>
       <c r="F176" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G176" s="29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H176" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C177" t="s">
+        <v>400</v>
       </c>
       <c r="D177" s="3"/>
       <c r="G177" s="29"/>
     </row>
-    <row r="178" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E178" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F178" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G178" s="29" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H178" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>39</v>
       </c>
       <c r="D179" s="3"/>
       <c r="G179" s="29"/>
     </row>
-    <row r="180" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>53</v>
-      </c>
-      <c r="D180" s="3"/>
-      <c r="G180" s="29"/>
-    </row>
-    <row r="181" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D180" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E180" t="s">
+        <v>79</v>
+      </c>
+      <c r="F180" t="s">
+        <v>371</v>
+      </c>
+      <c r="G180" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="H180" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>38</v>
-      </c>
-      <c r="C181" t="s">
-        <v>417</v>
+        <v>39</v>
       </c>
       <c r="D181" s="3"/>
       <c r="G181" s="29"/>
     </row>
-    <row r="182" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>38</v>
-      </c>
-      <c r="C182" t="s">
-        <v>475</v>
+        <v>53</v>
       </c>
       <c r="D182" s="3"/>
       <c r="G182" s="29"/>
     </row>
-    <row r="183" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>317</v>
-      </c>
+    <row r="183" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="C183" t="s">
+        <v>417</v>
       </c>
       <c r="D183" s="3"/>
       <c r="G183" s="29"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D184" s="18" t="s">
+    <row r="184" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>38</v>
+      </c>
+      <c r="C184" t="s">
+        <v>475</v>
+      </c>
+      <c r="D184" s="3"/>
+      <c r="G184" s="29"/>
+    </row>
+    <row r="185" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>317</v>
+      </c>
+      <c r="B185" t="s">
+        <v>52</v>
+      </c>
+      <c r="D185" s="3"/>
+      <c r="G185" s="29"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D186" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G184" s="27" t="s">
+      <c r="G186" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H184" s="16" t="s">
+      <c r="H186" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="185" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D185" s="3" t="s">
+    <row r="187" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D187" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G185" s="29" t="s">
+      <c r="G187" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H185" t="s">
+      <c r="H187" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D186" s="18" t="s">
+    <row r="188" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D188" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E186" s="16" t="s">
+      <c r="E188" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F186" s="16" t="s">
+      <c r="F188" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="G186" s="27" t="s">
+      <c r="G188" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="H186" s="18" t="s">
+      <c r="H188" s="18" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="16" t="s">
+    <row r="189" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C187" s="16" t="s">
+      <c r="C189" s="16" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D188" s="18" t="s">
+    <row r="190" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D190" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F188" s="16" t="s">
+      <c r="F190" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="G188" s="27" t="s">
+      <c r="G190" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H188" s="16" t="s">
+      <c r="H190" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D189" s="18" t="s">
+    <row r="191" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D191" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E191" t="s">
         <v>48</v>
       </c>
-      <c r="F189" s="27" t="s">
+      <c r="F191" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="G189" s="16"/>
-    </row>
-    <row r="190" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="16" t="s">
+      <c r="G191" s="16"/>
+    </row>
+    <row r="192" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C190" s="16" t="s">
+      <c r="C192" s="16" t="s">
         <v>383</v>
-      </c>
-      <c r="F190" s="27"/>
-      <c r="G190" s="16"/>
-    </row>
-    <row r="191" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D191" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F191" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="G191" s="16"/>
-      <c r="I191" s="16" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F192" s="27"/>
       <c r="G192" s="16"/>
     </row>
-    <row r="193" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="16" t="s">
+    <row r="193" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D193" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F193" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="G193" s="16"/>
+      <c r="I193" s="16" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="194" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F194" s="27"/>
+      <c r="G194" s="16"/>
+    </row>
+    <row r="195" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C193" s="16" t="s">
+      <c r="C195" s="16" t="s">
         <v>384</v>
-      </c>
-      <c r="F193" s="27"/>
-      <c r="G193" s="16"/>
-    </row>
-    <row r="194" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D194" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F194" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="G194" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H194" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="195" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="F195" s="27"/>
       <c r="G195" s="16"/>
     </row>
-    <row r="196" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="16" t="s">
+    <row r="196" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D196" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F196" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="G196" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H196" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="F196" s="27"/>
-      <c r="G196" s="16"/>
-    </row>
-    <row r="197" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F197" s="27"/>
       <c r="G197" s="16"/>
     </row>
-    <row r="198" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C198" s="16" t="s">
-        <v>318</v>
+        <v>39</v>
       </c>
       <c r="F198" s="27"/>
       <c r="G198" s="16"/>
     </row>
-    <row r="199" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
-        <v>52</v>
+    <row r="199" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B199" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="F199" s="27"/>
       <c r="G199" s="16"/>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D200" s="18" t="s">
+    <row r="200" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C200" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F200" s="27"/>
+      <c r="G200" s="16"/>
+    </row>
+    <row r="201" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>52</v>
+      </c>
+      <c r="F201" s="27"/>
+      <c r="G201" s="16"/>
+    </row>
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D202" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G200" s="27" t="s">
+      <c r="G202" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H200" s="16" t="s">
+      <c r="H202" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="201" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D201" s="3" t="s">
+    <row r="203" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D203" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E201" s="16" t="s">
+      <c r="E203" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F201" s="16" t="s">
+      <c r="F203" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="G201" s="27" t="s">
+      <c r="G203" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H201" s="16" t="s">
+      <c r="H203" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="202" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="16" t="s">
+    <row r="204" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
         <v>52</v>
       </c>
-      <c r="D203" s="3"/>
-    </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D204" s="18" t="s">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D206" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G204" s="27" t="s">
+      <c r="G206" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H204" s="16" t="s">
+      <c r="H206" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="205" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D205" s="18" t="s">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D207" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F205" s="16" t="s">
+      <c r="F207" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="G205" s="27" t="s">
+      <c r="G207" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="H205" s="16" t="s">
+      <c r="H207" s="16" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D206" s="18" t="s">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D208" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E206" s="16" t="s">
+      <c r="E208" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F206" s="16" t="s">
+      <c r="F208" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="G206" s="27" t="s">
+      <c r="G208" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H206" s="16" t="s">
+      <c r="H208" s="16" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B207" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C207" s="16" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D208" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F208" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="G208" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H208" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="209" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B209" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C209" s="16" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="210" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B210" s="16" t="s">
-        <v>53</v>
+      <c r="D210" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F210" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="G210" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H210" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="211" spans="2:16" x14ac:dyDescent="0.25">
@@ -4360,12 +4369,12 @@
     </row>
     <row r="212" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B212" s="16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="213" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B213" s="16" t="s">
-        <v>421</v>
+        <v>39</v>
       </c>
     </row>
     <row r="214" spans="2:16" x14ac:dyDescent="0.25">
@@ -4375,107 +4384,117 @@
     </row>
     <row r="215" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B215" s="16" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="216" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B216" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B217" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C215" s="16" t="s">
+      <c r="C217" s="16" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="216" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
+    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
         <v>52</v>
       </c>
-      <c r="D216" s="18"/>
-      <c r="E216" s="16"/>
-      <c r="F216" s="16"/>
-      <c r="G216" s="27"/>
-      <c r="H216" s="16"/>
-    </row>
-    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D217" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G217" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H217" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D218" s="18" t="s">
-        <v>40</v>
-      </c>
+      <c r="D218" s="18"/>
       <c r="E218" s="16"/>
       <c r="F218" s="16"/>
-      <c r="G218" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="H218" s="16" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="219" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G218" s="27"/>
+      <c r="H218" s="16"/>
+    </row>
+    <row r="219" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D219" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E219" s="16"/>
-      <c r="F219" s="16"/>
       <c r="G219" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H219" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D220" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E220" s="16"/>
+      <c r="F220" s="16"/>
+      <c r="G220" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="H220" s="16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D221" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E221" s="16"/>
+      <c r="F221" s="16"/>
+      <c r="G221" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="H219" s="16" t="s">
+      <c r="H221" s="16" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D220" t="s">
+    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D222" t="s">
         <v>73</v>
       </c>
-      <c r="F220" t="s">
+      <c r="F222" t="s">
         <v>240</v>
       </c>
-      <c r="G220" t="s">
+      <c r="G222" t="s">
         <v>405</v>
       </c>
-      <c r="H220" t="s">
+      <c r="H222" t="s">
         <v>406</v>
       </c>
-      <c r="O220" s="16"/>
-      <c r="P220" t="s">
+      <c r="O222" s="16"/>
+      <c r="P222" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D221" t="s">
+    <row r="223" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D223" t="s">
         <v>73</v>
       </c>
-      <c r="F221" t="s">
+      <c r="F223" t="s">
         <v>241</v>
       </c>
-      <c r="G221" t="s">
+      <c r="G223" t="s">
         <v>408</v>
       </c>
-      <c r="H221" t="s">
+      <c r="H223" t="s">
         <v>409</v>
       </c>
-      <c r="O221" s="16"/>
-      <c r="P221" t="s">
+      <c r="O223" s="16"/>
+      <c r="P223" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B222" t="s">
+    <row r="224" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="223" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B223" s="16" t="s">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="224" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B224" s="16" t="s">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4491,7 +4510,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A5:B7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4547,7 +4566,7 @@
   <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
@@ -6144,8 +6163,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6172,13 +6191,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -6186,13 +6205,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -6200,13 +6219,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -6214,13 +6233,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3" t="b">
+      <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -6228,13 +6247,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="3" t="b">
+      <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -6242,13 +6261,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>390</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="b">
+      <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -6256,13 +6275,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="b">
+      <c r="C8" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -6270,18 +6289,21 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="b">
+      <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="16"/>
@@ -6289,53 +6311,58 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="b">
+      <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>234</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="3" t="b">
+      <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" t="s">
         <v>372</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="b">
+      <c r="C13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" t="s">
         <v>375</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>242</v>
       </c>
       <c r="B16" t="s">
@@ -6346,7 +6373,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" t="s">
         <v>243</v>
       </c>
       <c r="B17" t="s">
@@ -6357,44 +6384,49 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="b">
+      <c r="C18" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="b">
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>232</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" t="s">
         <v>290</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" t="s">
         <v>37</v>
       </c>
       <c r="C22" t="b">
@@ -6402,10 +6434,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" t="s">
         <v>74</v>
       </c>
       <c r="C23" t="b">
@@ -6413,43 +6445,43 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" t="s">
         <v>292</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="3" t="b">
+      <c r="C24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="3" t="b">
+      <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" t="s">
         <v>294</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="3" t="b">
+      <c r="C26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" t="s">
         <v>364</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="b">
@@ -6457,46 +6489,48 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
       <c r="C28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" t="s">
         <v>280</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="3" t="b">
+      <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" t="s">
         <v>281</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="3" t="b">
+      <c r="C30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" t="s">
         <v>365</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="3" t="b">
+      <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" t="s">
         <v>366</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32" t="b">
@@ -6504,43 +6538,48 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" t="s">
         <v>367</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" t="s">
         <v>73</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+      <c r="A35" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="3" t="b">
+      <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="3" t="b">
+      <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="b">
@@ -6548,10 +6587,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
       <c r="C38" t="b">
@@ -6559,43 +6598,43 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="3" t="b">
+      <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="3" t="b">
+      <c r="C40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" t="s">
         <v>222</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="b">
+      <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" t="s">
         <v>289</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" t="s">
         <v>37</v>
       </c>
       <c r="C42" t="b">
@@ -6603,10 +6642,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" t="s">
         <v>225</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" t="s">
         <v>37</v>
       </c>
       <c r="C43" t="b">
@@ -6614,46 +6653,48 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" t="s">
         <v>227</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="3" t="b">
+      <c r="C44" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="3" t="b">
+      <c r="C45" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="3" t="b">
+      <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="B47"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" t="s">
         <v>295</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" t="s">
         <v>37</v>
       </c>
       <c r="C48" t="b">
@@ -6661,65 +6702,65 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" t="s">
         <v>297</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="3" t="b">
+      <c r="C49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" t="s">
         <v>376</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="3" t="b">
+      <c r="C50" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" t="s">
         <v>380</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="3" t="b">
+      <c r="C51" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" t="s">
         <v>298</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="3" t="b">
+      <c r="C52" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" t="s">
         <v>299</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="3" t="b">
+      <c r="C53" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" t="s">
         <v>302</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" t="s">
         <v>37</v>
       </c>
       <c r="C54" t="b">
@@ -6727,15 +6768,20 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" t="s">
         <v>304</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" t="s">
         <v>73</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -6744,7 +6790,7 @@
       <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="3" t="b">
+      <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6755,7 +6801,7 @@
       <c r="B58" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="3" t="b">
+      <c r="C58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6788,26 +6834,31 @@
       <c r="B61" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" t="s">
         <v>317</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="3" t="b">
+      <c r="C63" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" t="s">
         <v>319</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" t="s">
         <v>30</v>
       </c>
       <c r="C64" t="b">
@@ -6815,10 +6866,10 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" t="s">
         <v>386</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" t="s">
         <v>74</v>
       </c>
       <c r="C65" t="b">
@@ -6826,10 +6877,10 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
+      <c r="A66" t="s">
         <v>385</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" t="s">
         <v>76</v>
       </c>
       <c r="C66" t="b">
@@ -6837,7 +6888,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" t="s">
         <v>320</v>
       </c>
       <c r="B67" t="s">
@@ -6848,37 +6899,42 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="A68" t="s">
         <v>321</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" t="s">
         <v>73</v>
       </c>
-      <c r="C68" s="3" t="b">
+      <c r="C68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="A69" t="s">
         <v>322</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" t="s">
         <v>37</v>
       </c>
-      <c r="C69" s="3" t="b">
+      <c r="C69" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+      <c r="A70" t="s">
         <v>323</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" t="s">
         <v>73</v>
       </c>
-      <c r="C70" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -6972,13 +7028,13 @@
       <c r="D78"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" t="s">
         <v>153</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="3" t="b">
+      <c r="C79" t="b">
         <v>0</v>
       </c>
       <c r="D79" s="3" t="s">
@@ -6986,13 +7042,13 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
+      <c r="A80" t="s">
         <v>238</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="3" t="b">
+      <c r="C80" t="b">
         <v>0</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -7001,13 +7057,13 @@
       <c r="J80"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="A81" t="s">
         <v>239</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" t="s">
         <v>73</v>
       </c>
-      <c r="C81" s="3" t="b">
+      <c r="C81" t="b">
         <v>0</v>
       </c>
       <c r="G81"/>
@@ -7016,13 +7072,13 @@
       <c r="J81"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" t="s">
         <v>73</v>
       </c>
-      <c r="C82" s="3" t="b">
+      <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="G82"/>
@@ -7031,35 +7087,35 @@
       <c r="J82"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" t="s">
         <v>73</v>
       </c>
-      <c r="C83" s="3" t="b">
+      <c r="C83" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+      <c r="A84" t="s">
         <v>395</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="3" t="b">
+      <c r="C84" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
+      <c r="A85" t="s">
         <v>396</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" t="s">
         <v>73</v>
       </c>
-      <c r="C85" s="3" t="b">
+      <c r="C85" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed question on where cons + hosp
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788E350D-068A-4B7A-BA6E-E7FE9357E283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF79E29-B90B-40B0-AD60-B2C5E66DAE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="482">
   <si>
     <t>setting_name</t>
   </si>
@@ -1473,6 +1473,12 @@
   </si>
   <si>
     <t xml:space="preserve">data("EVENT") === "OLD QUESTION REMOVED 021120" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("CONS") === "OLD QUESTION REMOVED 021120" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("HOSP") === "OLD QUESTION REMOVED 021120" </t>
   </si>
 </sst>
 </file>
@@ -2029,11 +2035,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:P226"/>
+  <dimension ref="A1:P230"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,7 +3747,7 @@
         <v>38</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>296</v>
+        <v>480</v>
       </c>
       <c r="F152" s="27"/>
       <c r="G152" s="16"/>
@@ -3789,83 +3795,89 @@
     </row>
     <row r="157" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G157" s="16"/>
+    </row>
+    <row r="158" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C158" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F158" s="27"/>
+      <c r="G158" s="16"/>
+    </row>
+    <row r="159" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F157" s="27"/>
-      <c r="G157" s="16"/>
-    </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D158" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G158" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H158" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D159" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F159" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="G159" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="H159" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F159" s="27"/>
+      <c r="G159" s="16"/>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D160" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E160" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>302</v>
+        <v>40</v>
       </c>
       <c r="G160" s="27" t="s">
-        <v>307</v>
+        <v>133</v>
       </c>
       <c r="H160" s="16" t="s">
-        <v>308</v>
+        <v>134</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B161" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C161" s="16" t="s">
-        <v>303</v>
+      <c r="D161" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="H161" s="16" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D162" s="18" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="E162" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="F162" s="16" t="s">
-        <v>304</v>
-      </c>
-      <c r="G162" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H162" t="s">
-        <v>306</v>
+        <v>302</v>
+      </c>
+      <c r="G162" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="H162" s="16" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B163" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C163" s="16" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B164" s="16" t="s">
-        <v>53</v>
+      <c r="D164" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="G164" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H164" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -3873,117 +3885,100 @@
         <v>39</v>
       </c>
     </row>
-    <row r="166" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B167" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>78</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B168" t="s">
         <v>52</v>
       </c>
-      <c r="D166" s="3"/>
-      <c r="G166" s="29"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D167" s="18" t="s">
+      <c r="D168" s="3"/>
+      <c r="G168" s="29"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D169" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G167" s="27" t="s">
+      <c r="G169" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H167" s="16" t="s">
+      <c r="H169" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="168" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D168" s="3" t="s">
+    <row r="170" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D170" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G168" s="29" t="s">
+      <c r="G170" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H168" t="s">
+      <c r="H170" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="169" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D169" s="3" t="s">
+    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D171" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E171" t="s">
         <v>59</v>
       </c>
-      <c r="F169" t="s">
+      <c r="F171" t="s">
         <v>78</v>
       </c>
-      <c r="G169" s="29" t="s">
+      <c r="G171" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="H169" t="s">
+      <c r="H171" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="170" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B170" t="s">
+    <row r="172" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>53</v>
       </c>
-      <c r="D170" s="3"/>
-      <c r="G170" s="29"/>
-    </row>
-    <row r="171" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
+      <c r="D172" s="3"/>
+      <c r="G172" s="29"/>
+    </row>
+    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
         <v>52</v>
       </c>
-      <c r="D171" s="3"/>
-      <c r="G171" s="29"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D172" s="18" t="s">
+      <c r="D173" s="3"/>
+      <c r="G173" s="29"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D174" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G172" s="27" t="s">
+      <c r="G174" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H172" s="16" t="s">
+      <c r="H174" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="173" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D173" s="3" t="s">
+    <row r="175" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D175" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G173" s="29" t="s">
+      <c r="G175" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H173" t="s">
+      <c r="H175" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D174" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E174" t="s">
-        <v>59</v>
-      </c>
-      <c r="F174" t="s">
-        <v>368</v>
-      </c>
-      <c r="G174" s="29" t="s">
-        <v>459</v>
-      </c>
-      <c r="H174" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B175" t="s">
-        <v>38</v>
-      </c>
-      <c r="C175" t="s">
-        <v>399</v>
-      </c>
-      <c r="D175" s="3"/>
-      <c r="G175" s="29"/>
     </row>
     <row r="176" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D176" s="3" t="s">
@@ -3993,13 +3988,13 @@
         <v>59</v>
       </c>
       <c r="F176" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G176" s="29" t="s">
-        <v>311</v>
+        <v>459</v>
       </c>
       <c r="H176" t="s">
-        <v>312</v>
+        <v>460</v>
       </c>
     </row>
     <row r="177" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4007,47 +4002,50 @@
         <v>38</v>
       </c>
       <c r="C177" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D177" s="3"/>
       <c r="G177" s="29"/>
     </row>
     <row r="178" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" s="3" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="E178" t="s">
+        <v>59</v>
       </c>
       <c r="F178" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G178" s="29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H178" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="179" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C179" t="s">
+        <v>400</v>
       </c>
       <c r="D179" s="3"/>
       <c r="G179" s="29"/>
     </row>
     <row r="180" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D180" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E180" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F180" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G180" s="29" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H180" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="181" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4058,443 +4056,482 @@
       <c r="G181" s="29"/>
     </row>
     <row r="182" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>53</v>
-      </c>
-      <c r="D182" s="3"/>
-      <c r="G182" s="29"/>
+      <c r="D182" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E182" t="s">
+        <v>79</v>
+      </c>
+      <c r="F182" t="s">
+        <v>371</v>
+      </c>
+      <c r="G182" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="H182" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="183" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>38</v>
-      </c>
-      <c r="C183" t="s">
-        <v>417</v>
+        <v>39</v>
       </c>
       <c r="D183" s="3"/>
       <c r="G183" s="29"/>
     </row>
     <row r="184" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>38</v>
-      </c>
-      <c r="C184" t="s">
-        <v>475</v>
+        <v>53</v>
       </c>
       <c r="D184" s="3"/>
       <c r="G184" s="29"/>
     </row>
     <row r="185" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>317</v>
-      </c>
       <c r="B185" t="s">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="C185" t="s">
+        <v>417</v>
       </c>
       <c r="D185" s="3"/>
       <c r="G185" s="29"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D186" s="18" t="s">
+    <row r="186" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>38</v>
+      </c>
+      <c r="C186" t="s">
+        <v>475</v>
+      </c>
+      <c r="D186" s="3"/>
+      <c r="G186" s="29"/>
+    </row>
+    <row r="187" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>317</v>
+      </c>
+      <c r="B187" t="s">
+        <v>52</v>
+      </c>
+      <c r="D187" s="3"/>
+      <c r="G187" s="29"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D188" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G186" s="27" t="s">
+      <c r="G188" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H186" s="16" t="s">
+      <c r="H188" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="187" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D187" s="3" t="s">
+    <row r="189" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D189" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G187" s="29" t="s">
+      <c r="G189" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H187" t="s">
+      <c r="H189" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D188" s="18" t="s">
+    <row r="190" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D190" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E188" s="16" t="s">
+      <c r="E190" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F188" s="16" t="s">
+      <c r="F190" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="G188" s="27" t="s">
+      <c r="G190" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="H188" s="18" t="s">
+      <c r="H190" s="18" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="16" t="s">
+    <row r="191" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C189" s="16" t="s">
+      <c r="C191" s="16" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D190" s="18" t="s">
+    <row r="192" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D192" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F190" s="16" t="s">
+      <c r="F192" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="G190" s="27" t="s">
+      <c r="G192" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H190" s="16" t="s">
+      <c r="H192" s="16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D191" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E191" t="s">
-        <v>48</v>
-      </c>
-      <c r="F191" s="27" t="s">
-        <v>386</v>
-      </c>
-      <c r="G191" s="16"/>
-    </row>
-    <row r="192" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C192" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="F192" s="27"/>
-      <c r="G192" s="16"/>
     </row>
     <row r="193" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D193" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="E193" t="s">
+        <v>48</v>
       </c>
       <c r="F193" s="27" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="G193" s="16"/>
-      <c r="I193" s="16" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="194" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C194" s="16" t="s">
+        <v>383</v>
       </c>
       <c r="F194" s="27"/>
       <c r="G194" s="16"/>
     </row>
     <row r="195" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C195" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="F195" s="27"/>
+      <c r="D195" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F195" s="27" t="s">
+        <v>319</v>
+      </c>
       <c r="G195" s="16"/>
+      <c r="I195" s="16" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="196" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D196" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F196" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="G196" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H196" s="16" t="s">
-        <v>382</v>
-      </c>
+      <c r="B196" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F196" s="27"/>
+      <c r="G196" s="16"/>
     </row>
     <row r="197" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C197" s="16" t="s">
+        <v>384</v>
       </c>
       <c r="F197" s="27"/>
       <c r="G197" s="16"/>
     </row>
     <row r="198" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F198" s="27"/>
-      <c r="G198" s="16"/>
+      <c r="D198" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F198" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="G198" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H198" s="16" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="199" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F199" s="27"/>
       <c r="G199" s="16"/>
     </row>
     <row r="200" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C200" s="16" t="s">
-        <v>318</v>
+        <v>39</v>
       </c>
       <c r="F200" s="27"/>
       <c r="G200" s="16"/>
     </row>
     <row r="201" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>52</v>
+      <c r="B201" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="F201" s="27"/>
       <c r="G201" s="16"/>
     </row>
-    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D202" s="18" t="s">
+    <row r="202" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C202" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="F202" s="27"/>
+      <c r="G202" s="16"/>
+    </row>
+    <row r="203" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>52</v>
+      </c>
+      <c r="F203" s="27"/>
+      <c r="G203" s="16"/>
+    </row>
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D204" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G202" s="27" t="s">
+      <c r="G204" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H202" s="16" t="s">
+      <c r="H204" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="203" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D203" s="3" t="s">
+    <row r="205" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D205" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E203" s="16" t="s">
+      <c r="E205" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F203" s="16" t="s">
+      <c r="F205" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="G203" s="27" t="s">
+      <c r="G205" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H203" s="16" t="s">
+      <c r="H205" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="204" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="16" t="s">
+    <row r="206" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D204" s="3"/>
-    </row>
-    <row r="205" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" t="s">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B208" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C208" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
         <v>52</v>
       </c>
-      <c r="D205" s="3"/>
-    </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D206" s="18" t="s">
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D210" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G206" s="27" t="s">
+      <c r="G210" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H206" s="16" t="s">
+      <c r="H210" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D207" s="18" t="s">
+    <row r="211" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D211" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F207" s="16" t="s">
+      <c r="F211" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="G207" s="27" t="s">
+      <c r="G211" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="H207" s="16" t="s">
+      <c r="H211" s="16" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D208" s="18" t="s">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D212" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E208" s="16" t="s">
+      <c r="E212" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F208" s="16" t="s">
+      <c r="F212" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="G208" s="27" t="s">
+      <c r="G212" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="H208" s="16" t="s">
+      <c r="H212" s="16" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="209" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B209" s="16" t="s">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B213" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C209" s="16" t="s">
+      <c r="C213" s="16" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="210" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D210" s="18" t="s">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D214" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F210" s="16" t="s">
+      <c r="F214" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="G210" s="29" t="s">
+      <c r="G214" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="H210" t="s">
+      <c r="H214" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="211" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B211" s="16" t="s">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B215" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="212" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B212" s="16" t="s">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B216" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="213" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B213" s="16" t="s">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B217" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="214" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B214" s="16" t="s">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B218" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="215" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B215" s="16" t="s">
+    <row r="219" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B219" s="16" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="216" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B216" s="16" t="s">
+    <row r="220" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B220" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="217" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B217" s="16" t="s">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B221" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C217" s="16" t="s">
+      <c r="C221" s="16" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="218" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
+    <row r="222" spans="2:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
         <v>52</v>
       </c>
-      <c r="D218" s="18"/>
-      <c r="E218" s="16"/>
-      <c r="F218" s="16"/>
-      <c r="G218" s="27"/>
-      <c r="H218" s="16"/>
-    </row>
-    <row r="219" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D219" s="18" t="s">
+      <c r="D222" s="18"/>
+      <c r="E222" s="16"/>
+      <c r="F222" s="16"/>
+      <c r="G222" s="27"/>
+      <c r="H222" s="16"/>
+    </row>
+    <row r="223" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D223" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G219" s="27" t="s">
+      <c r="G223" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="H219" s="16" t="s">
+      <c r="H223" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="220" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D220" s="18" t="s">
+    <row r="224" spans="2:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D224" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E220" s="16"/>
-      <c r="F220" s="16"/>
-      <c r="G220" s="27" t="s">
+      <c r="E224" s="16"/>
+      <c r="F224" s="16"/>
+      <c r="G224" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H220" s="16" t="s">
+      <c r="H224" s="16" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="221" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D221" s="18" t="s">
+    <row r="225" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D225" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E221" s="16"/>
-      <c r="F221" s="16"/>
-      <c r="G221" s="27" t="s">
+      <c r="E225" s="16"/>
+      <c r="F225" s="16"/>
+      <c r="G225" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="H221" s="16" t="s">
+      <c r="H225" s="16" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="222" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D222" t="s">
+    <row r="226" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
         <v>73</v>
       </c>
-      <c r="F222" t="s">
+      <c r="F226" t="s">
         <v>240</v>
       </c>
-      <c r="G222" t="s">
+      <c r="G226" t="s">
         <v>405</v>
       </c>
-      <c r="H222" t="s">
+      <c r="H226" t="s">
         <v>406</v>
       </c>
-      <c r="O222" s="16"/>
-      <c r="P222" t="s">
+      <c r="O226" s="16"/>
+      <c r="P226" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="223" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D223" t="s">
+    <row r="227" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D227" t="s">
         <v>73</v>
       </c>
-      <c r="F223" t="s">
+      <c r="F227" t="s">
         <v>241</v>
       </c>
-      <c r="G223" t="s">
+      <c r="G227" t="s">
         <v>408</v>
       </c>
-      <c r="H223" t="s">
+      <c r="H227" t="s">
         <v>409</v>
       </c>
-      <c r="O223" s="16"/>
-      <c r="P223" t="s">
+      <c r="O227" s="16"/>
+      <c r="P227" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="224" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B224" t="s">
+    <row r="228" spans="2:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B225" s="16" t="s">
+    <row r="229" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B229" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B226" s="16" t="s">
+    <row r="230" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B230" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6162,7 +6199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:C85"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Suzete to assistants
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8DF83-3E98-43BD-A89B-5929A1248116}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE2E83C-E0CF-42E6-96CA-A2FAADC701CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="505">
   <si>
     <t>setting_name</t>
   </si>
@@ -1542,6 +1542,12 @@
   </si>
   <si>
     <t>Randomization variable</t>
+  </si>
+  <si>
+    <t>SUZ</t>
+  </si>
+  <si>
+    <t>Suzete</t>
   </si>
 </sst>
 </file>
@@ -1978,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
@@ -4693,11 +4699,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,40 +4938,39 @@
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="B18" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>143</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" t="s">
+        <v>503</v>
+      </c>
+      <c r="C17" t="s">
+        <v>504</v>
+      </c>
+      <c r="D17" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>416</v>
       </c>
       <c r="B19" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4973,14 +4978,14 @@
         <v>416</v>
       </c>
       <c r="B20" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4988,14 +4993,14 @@
         <v>416</v>
       </c>
       <c r="B21" t="str">
-        <f>"4"</f>
-        <v>4</v>
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>460</v>
+        <v>145</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>461</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5003,117 +5008,117 @@
         <v>416</v>
       </c>
       <c r="B22" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="B23" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
     <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
       <c r="B25" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>251</v>
-      </c>
+    <row r="27" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>249</v>
       </c>
       <c r="B28" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F28" s="16"/>
+        <v>250</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>249</v>
       </c>
       <c r="B29" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>255</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>249</v>
       </c>
-      <c r="B30" s="12" t="str">
-        <f>"4"</f>
-        <v>4</v>
+      <c r="B30" t="str">
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5121,14 +5126,14 @@
         <v>249</v>
       </c>
       <c r="B31" s="12" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -5136,14 +5141,14 @@
         <v>249</v>
       </c>
       <c r="B32" s="12" t="str">
-        <f>"6"</f>
-        <v>6</v>
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>421</v>
+        <v>258</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>423</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5151,44 +5156,44 @@
         <v>249</v>
       </c>
       <c r="B33" s="12" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="12" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>158</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B36" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>267</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5196,29 +5201,29 @@
         <v>158</v>
       </c>
       <c r="B37" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="12" t="str">
-        <f>"2"</f>
-        <v>2</v>
+      <c r="B38" t="str">
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>329</v>
+        <v>161</v>
       </c>
       <c r="D38" t="s">
-        <v>328</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5226,50 +5231,50 @@
         <v>158</v>
       </c>
       <c r="B39" s="12" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>329</v>
+      </c>
+      <c r="D39" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="12" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>163</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>59</v>
       </c>
       <c r="B42" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5277,47 +5282,47 @@
         <v>59</v>
       </c>
       <c r="B43" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>48</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B46" t="str">
         <f>"D:NS,M:NS,Y:NS"</f>
         <v>D:NS,M:NS,Y:NS</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5325,14 +5330,14 @@
         <v>79</v>
       </c>
       <c r="B48" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -5340,47 +5345,47 @@
         <v>79</v>
       </c>
       <c r="B49" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="7" t="str">
-        <f>"301"</f>
-        <v>301</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>168</v>
-      </c>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="13" t="str">
-        <f>"304"</f>
-        <v>304</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>89</v>
+      <c r="B52" s="7" t="str">
+        <f>"301"</f>
+        <v>301</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -5388,14 +5393,14 @@
         <v>88</v>
       </c>
       <c r="B53" s="13" t="str">
-        <f>"305"</f>
-        <v>305</v>
+        <f>"304"</f>
+        <v>304</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5403,14 +5408,14 @@
         <v>88</v>
       </c>
       <c r="B54" s="13" t="str">
-        <f>"306"</f>
-        <v>306</v>
+        <f>"305"</f>
+        <v>305</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5418,14 +5423,14 @@
         <v>88</v>
       </c>
       <c r="B55" s="13" t="str">
-        <f>"307"</f>
-        <v>307</v>
+        <f>"306"</f>
+        <v>306</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5433,14 +5438,14 @@
         <v>88</v>
       </c>
       <c r="B56" s="13" t="str">
-        <f>"308"</f>
-        <v>308</v>
+        <f>"307"</f>
+        <v>307</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5448,14 +5453,14 @@
         <v>88</v>
       </c>
       <c r="B57" s="13" t="str">
-        <f>"309"</f>
-        <v>309</v>
+        <f>"308"</f>
+        <v>308</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5463,14 +5468,14 @@
         <v>88</v>
       </c>
       <c r="B58" s="13" t="str">
-        <f>"310"</f>
-        <v>310</v>
+        <f>"309"</f>
+        <v>309</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>169</v>
+        <v>94</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>169</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5478,14 +5483,14 @@
         <v>88</v>
       </c>
       <c r="B59" s="13" t="str">
-        <f>"311"</f>
-        <v>311</v>
+        <f>"310"</f>
+        <v>310</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,14 +5498,14 @@
         <v>88</v>
       </c>
       <c r="B60" s="13" t="str">
-        <f>"312"</f>
-        <v>312</v>
+        <f>"311"</f>
+        <v>311</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5508,14 +5513,14 @@
         <v>88</v>
       </c>
       <c r="B61" s="13" t="str">
-        <f>"313"</f>
-        <v>313</v>
+        <f>"312"</f>
+        <v>312</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5523,14 +5528,14 @@
         <v>88</v>
       </c>
       <c r="B62" s="13" t="str">
-        <f>"314"</f>
-        <v>314</v>
+        <f>"313"</f>
+        <v>313</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -5538,14 +5543,14 @@
         <v>88</v>
       </c>
       <c r="B63" s="13" t="str">
-        <f>"315"</f>
-        <v>315</v>
+        <f>"314"</f>
+        <v>314</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5553,14 +5558,14 @@
         <v>88</v>
       </c>
       <c r="B64" s="13" t="str">
-        <f>"316"</f>
-        <v>316</v>
+        <f>"315"</f>
+        <v>315</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -5568,14 +5573,14 @@
         <v>88</v>
       </c>
       <c r="B65" s="13" t="str">
-        <f>"317"</f>
-        <v>317</v>
+        <f>"316"</f>
+        <v>316</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -5583,14 +5588,14 @@
         <v>88</v>
       </c>
       <c r="B66" s="13" t="str">
-        <f>"318"</f>
-        <v>318</v>
+        <f>"317"</f>
+        <v>317</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -5598,14 +5603,14 @@
         <v>88</v>
       </c>
       <c r="B67" s="13" t="str">
-        <f>"319"</f>
-        <v>319</v>
+        <f>"318"</f>
+        <v>318</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -5613,14 +5618,14 @@
         <v>88</v>
       </c>
       <c r="B68" s="13" t="str">
-        <f>"320"</f>
-        <v>320</v>
+        <f>"319"</f>
+        <v>319</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -5628,14 +5633,14 @@
         <v>88</v>
       </c>
       <c r="B69" s="13" t="str">
-        <f>"321"</f>
-        <v>321</v>
+        <f>"320"</f>
+        <v>320</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -5643,14 +5648,14 @@
         <v>88</v>
       </c>
       <c r="B70" s="13" t="str">
-        <f>"322"</f>
-        <v>322</v>
+        <f>"321"</f>
+        <v>321</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -5658,14 +5663,14 @@
         <v>88</v>
       </c>
       <c r="B71" s="13" t="str">
-        <f>"323"</f>
-        <v>323</v>
+        <f>"322"</f>
+        <v>322</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -5673,14 +5678,14 @@
         <v>88</v>
       </c>
       <c r="B72" s="13" t="str">
-        <f>"324"</f>
-        <v>324</v>
+        <f>"323"</f>
+        <v>323</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -5688,47 +5693,47 @@
         <v>88</v>
       </c>
       <c r="B73" s="13" t="str">
+        <f>"324"</f>
+        <v>324</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>88</v>
+      </c>
+      <c r="B74" s="13" t="str">
         <f>"325"</f>
         <v>325</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C74" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="D74" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="7"/>
-    </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>173</v>
-      </c>
-      <c r="B75" s="7" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="B75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>173</v>
       </c>
       <c r="B76" s="7" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>176</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -5736,14 +5741,14 @@
         <v>173</v>
       </c>
       <c r="B77" s="7" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C77" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>177</v>
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -5751,14 +5756,14 @@
         <v>173</v>
       </c>
       <c r="B78" s="7" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C78" s="21" t="s">
-        <v>178</v>
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -5766,14 +5771,14 @@
         <v>173</v>
       </c>
       <c r="B79" s="7" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C79" s="23" t="s">
-        <v>180</v>
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -5781,14 +5786,14 @@
         <v>173</v>
       </c>
       <c r="B80" s="7" t="str">
-        <f>"6"</f>
-        <v>6</v>
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -5796,14 +5801,14 @@
         <v>173</v>
       </c>
       <c r="B81" s="7" t="str">
-        <f>"7"</f>
-        <v>7</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>243</v>
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>182</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -5811,14 +5816,14 @@
         <v>173</v>
       </c>
       <c r="B82" s="7" t="str">
-        <f>"8"</f>
-        <v>8</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>185</v>
+        <f>"7"</f>
+        <v>7</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -5826,14 +5831,14 @@
         <v>173</v>
       </c>
       <c r="B83" s="7" t="str">
-        <f>"9"</f>
-        <v>9</v>
+        <f>"8"</f>
+        <v>8</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -5841,14 +5846,14 @@
         <v>173</v>
       </c>
       <c r="B84" s="7" t="str">
-        <f>"11"</f>
-        <v>11</v>
+        <f>"9"</f>
+        <v>9</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>424</v>
+        <v>187</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>425</v>
+        <v>188</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -5856,14 +5861,14 @@
         <v>173</v>
       </c>
       <c r="B85" s="7" t="str">
-        <f>"12"</f>
-        <v>12</v>
+        <f>"11"</f>
+        <v>11</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>452</v>
+        <v>424</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -5871,48 +5876,48 @@
         <v>173</v>
       </c>
       <c r="B86" s="7" t="str">
+        <f>"12"</f>
+        <v>12</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>452</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>173</v>
+      </c>
+      <c r="B87" s="7" t="str">
         <f>"10"</f>
         <v>10</v>
       </c>
-      <c r="C86" s="23" t="s">
+      <c r="C87" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D87" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="7"/>
-      <c r="C87" s="23"/>
-    </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>191</v>
-      </c>
-      <c r="B88" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C88" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="B88" s="7"/>
+      <c r="C88" s="23"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>191</v>
       </c>
       <c r="B89" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -5920,14 +5925,14 @@
         <v>191</v>
       </c>
       <c r="B90" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>454</v>
+        <v>194</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>455</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -5935,97 +5940,97 @@
         <v>191</v>
       </c>
       <c r="B91" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>196</v>
+        <v>454</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>197</v>
+        <v>455</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>191</v>
       </c>
-      <c r="B92" s="7" t="str">
+      <c r="B92" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>191</v>
+      </c>
+      <c r="B93" s="7" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C92" s="23" t="s">
+      <c r="C93" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="7"/>
-      <c r="C93" s="23"/>
-    </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>200</v>
-      </c>
-      <c r="B94" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C94" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="B94" s="7"/>
+      <c r="C94" s="23"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>200</v>
       </c>
       <c r="B95" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C95" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>200</v>
+      </c>
+      <c r="B96" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C96" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="7"/>
-      <c r="C96" s="23"/>
-    </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>205</v>
-      </c>
-      <c r="B97" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C97" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>206</v>
-      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="23"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>205</v>
       </c>
       <c r="B98" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -6033,48 +6038,48 @@
         <v>205</v>
       </c>
       <c r="B99" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="C100" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="7"/>
-      <c r="C100" s="23"/>
-    </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>210</v>
-      </c>
-      <c r="B101" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C101" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>261</v>
-      </c>
+      <c r="B101" s="7"/>
+      <c r="C101" s="23"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>210</v>
       </c>
       <c r="B102" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>190</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -6082,48 +6087,48 @@
         <v>210</v>
       </c>
       <c r="B103" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C103" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="7"/>
-      <c r="C104" s="23"/>
-    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>214</v>
-      </c>
-      <c r="B105" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C105" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>217</v>
-      </c>
+      <c r="B105" s="7"/>
+      <c r="C105" s="23"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>214</v>
       </c>
       <c r="B106" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -6131,14 +6136,14 @@
         <v>214</v>
       </c>
       <c r="B107" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>467</v>
+        <v>236</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>466</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -6146,47 +6151,47 @@
         <v>214</v>
       </c>
       <c r="B108" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>214</v>
+      </c>
+      <c r="B109" t="str">
         <f>"6"</f>
         <v>6</v>
       </c>
-      <c r="C108" s="23" t="s">
+      <c r="C109" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C109" s="23"/>
-    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>479</v>
-      </c>
-      <c r="B110" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C110" s="23" t="s">
-        <v>480</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>483</v>
-      </c>
+      <c r="C110" s="23"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>479</v>
       </c>
       <c r="B111" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -6194,48 +6199,48 @@
         <v>479</v>
       </c>
       <c r="B112" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C112" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>479</v>
+      </c>
+      <c r="B113" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C112" s="23" t="s">
+      <c r="C113" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="7"/>
-      <c r="C113" s="23"/>
-    </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>218</v>
-      </c>
-      <c r="B114" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C114" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="B114" s="7"/>
+      <c r="C114" s="23"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>218</v>
       </c>
       <c r="B115" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C115" s="24" t="s">
-        <v>219</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>232</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -6243,14 +6248,14 @@
         <v>218</v>
       </c>
       <c r="B116" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>463</v>
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C116" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>465</v>
+        <v>221</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -6258,18 +6263,30 @@
         <v>218</v>
       </c>
       <c r="B117" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D118" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="7"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B119" s="7"/>
@@ -6318,6 +6335,9 @@
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Added Assistant 1 + 2 + Suzette to FU
</commit_message>
<xml_diff>
--- a/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
+++ b/app/config/tables/MASKFU/Forms/MASKFU/MASKFU.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE2E83C-E0CF-42E6-96CA-A2FAADC701CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4673E55F-41C7-4CDC-8FC6-A6F0485B52F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="509">
   <si>
     <t>setting_name</t>
   </si>
@@ -1548,6 +1548,18 @@
   </si>
   <si>
     <t>Suzete</t>
+  </si>
+  <si>
+    <t>AS1</t>
+  </si>
+  <si>
+    <t>AS2</t>
+  </si>
+  <si>
+    <t>Assistente 1</t>
+  </si>
+  <si>
+    <t>Assistente 2</t>
   </si>
 </sst>
 </file>
@@ -4699,11 +4711,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,55 +4964,53 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="B19" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>416</v>
-      </c>
-      <c r="B20" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>118</v>
-      </c>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C18" t="s">
+        <v>507</v>
+      </c>
+      <c r="D18" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" t="s">
+        <v>506</v>
+      </c>
+      <c r="C19" t="s">
+        <v>508</v>
+      </c>
+      <c r="D19" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>416</v>
       </c>
       <c r="B21" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5008,14 +5018,14 @@
         <v>416</v>
       </c>
       <c r="B22" t="str">
-        <f>"4"</f>
-        <v>4</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>460</v>
+        <v>117</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>461</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -5023,132 +5033,132 @@
         <v>416</v>
       </c>
       <c r="B23" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="B24" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="B25" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D25" s="12" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B27" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B28" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>249</v>
-      </c>
-      <c r="B28" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>249</v>
-      </c>
-      <c r="B29" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F29" s="16"/>
+    <row r="29" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>249</v>
       </c>
       <c r="B30" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>249</v>
       </c>
-      <c r="B31" s="12" t="str">
-        <f>"4"</f>
-        <v>4</v>
+      <c r="B31" t="str">
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>257</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>249</v>
       </c>
-      <c r="B32" s="12" t="str">
-        <f>"5"</f>
-        <v>5</v>
+      <c r="B32" t="str">
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5156,14 +5166,14 @@
         <v>249</v>
       </c>
       <c r="B33" s="12" t="str">
-        <f>"6"</f>
-        <v>6</v>
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>421</v>
+        <v>256</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>423</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5171,188 +5181,188 @@
         <v>249</v>
       </c>
       <c r="B34" s="12" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" s="12" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="12" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>158</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B38" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>267</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>158</v>
-      </c>
-      <c r="B37" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>158</v>
-      </c>
-      <c r="B38" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="12" t="str">
-        <f>"2"</f>
-        <v>2</v>
+      <c r="B39" t="str">
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>329</v>
+        <v>159</v>
       </c>
       <c r="D39" t="s">
-        <v>328</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="12" t="str">
+      <c r="B40" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="12" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>329</v>
+      </c>
+      <c r="D41" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="12" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>163</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>43</v>
-      </c>
+    <row r="43" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>59</v>
       </c>
       <c r="B44" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B46" t="str">
+      <c r="B48" t="str">
         <f>"D:NS,M:NS,Y:NS"</f>
         <v>D:NS,M:NS,Y:NS</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>79</v>
-      </c>
-      <c r="B48" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -5360,62 +5370,62 @@
         <v>79</v>
       </c>
       <c r="B50" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="7" t="str">
-        <f>"301"</f>
-        <v>301</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="13" t="str">
-        <f>"304"</f>
-        <v>304</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>89</v>
-      </c>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="13" t="str">
-        <f>"305"</f>
-        <v>305</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>90</v>
+      <c r="B54" s="7" t="str">
+        <f>"301"</f>
+        <v>301</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5423,14 +5433,14 @@
         <v>88</v>
       </c>
       <c r="B55" s="13" t="str">
-        <f>"306"</f>
-        <v>306</v>
+        <f>"304"</f>
+        <v>304</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5438,14 +5448,14 @@
         <v>88</v>
       </c>
       <c r="B56" s="13" t="str">
-        <f>"307"</f>
-        <v>307</v>
+        <f>"305"</f>
+        <v>305</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5453,14 +5463,14 @@
         <v>88</v>
       </c>
       <c r="B57" s="13" t="str">
-        <f>"308"</f>
-        <v>308</v>
+        <f>"306"</f>
+        <v>306</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5468,14 +5478,14 @@
         <v>88</v>
       </c>
       <c r="B58" s="13" t="str">
-        <f>"309"</f>
-        <v>309</v>
+        <f>"307"</f>
+        <v>307</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5483,14 +5493,14 @@
         <v>88</v>
       </c>
       <c r="B59" s="13" t="str">
-        <f>"310"</f>
-        <v>310</v>
+        <f>"308"</f>
+        <v>308</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5498,14 +5508,14 @@
         <v>88</v>
       </c>
       <c r="B60" s="13" t="str">
-        <f>"311"</f>
-        <v>311</v>
+        <f>"309"</f>
+        <v>309</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5513,14 +5523,14 @@
         <v>88</v>
       </c>
       <c r="B61" s="13" t="str">
-        <f>"312"</f>
-        <v>312</v>
+        <f>"310"</f>
+        <v>310</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>96</v>
+        <v>169</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>96</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5528,14 +5538,14 @@
         <v>88</v>
       </c>
       <c r="B62" s="13" t="str">
-        <f>"313"</f>
-        <v>313</v>
+        <f>"311"</f>
+        <v>311</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -5543,14 +5553,14 @@
         <v>88</v>
       </c>
       <c r="B63" s="13" t="str">
-        <f>"314"</f>
-        <v>314</v>
+        <f>"312"</f>
+        <v>312</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5558,14 +5568,14 @@
         <v>88</v>
       </c>
       <c r="B64" s="13" t="str">
-        <f>"315"</f>
-        <v>315</v>
+        <f>"313"</f>
+        <v>313</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -5573,14 +5583,14 @@
         <v>88</v>
       </c>
       <c r="B65" s="13" t="str">
-        <f>"316"</f>
-        <v>316</v>
+        <f>"314"</f>
+        <v>314</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -5588,14 +5598,14 @@
         <v>88</v>
       </c>
       <c r="B66" s="13" t="str">
-        <f>"317"</f>
-        <v>317</v>
+        <f>"315"</f>
+        <v>315</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -5603,14 +5613,14 @@
         <v>88</v>
       </c>
       <c r="B67" s="13" t="str">
-        <f>"318"</f>
-        <v>318</v>
+        <f>"316"</f>
+        <v>316</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -5618,14 +5628,14 @@
         <v>88</v>
       </c>
       <c r="B68" s="13" t="str">
-        <f>"319"</f>
-        <v>319</v>
+        <f>"317"</f>
+        <v>317</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -5633,14 +5643,14 @@
         <v>88</v>
       </c>
       <c r="B69" s="13" t="str">
-        <f>"320"</f>
-        <v>320</v>
+        <f>"318"</f>
+        <v>318</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -5648,14 +5658,14 @@
         <v>88</v>
       </c>
       <c r="B70" s="13" t="str">
-        <f>"321"</f>
-        <v>321</v>
+        <f>"319"</f>
+        <v>319</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -5663,14 +5673,14 @@
         <v>88</v>
       </c>
       <c r="B71" s="13" t="str">
-        <f>"322"</f>
-        <v>322</v>
+        <f>"320"</f>
+        <v>320</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -5678,14 +5688,14 @@
         <v>88</v>
       </c>
       <c r="B72" s="13" t="str">
-        <f>"323"</f>
-        <v>323</v>
+        <f>"321"</f>
+        <v>321</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -5693,14 +5703,14 @@
         <v>88</v>
       </c>
       <c r="B73" s="13" t="str">
-        <f>"324"</f>
-        <v>324</v>
+        <f>"322"</f>
+        <v>322</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -5708,62 +5718,62 @@
         <v>88</v>
       </c>
       <c r="B74" s="13" t="str">
+        <f>"323"</f>
+        <v>323</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="13" t="str">
+        <f>"324"</f>
+        <v>324</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" s="13" t="str">
         <f>"325"</f>
         <v>325</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C76" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D76" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="7"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>173</v>
-      </c>
-      <c r="B76" s="7" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>173</v>
-      </c>
-      <c r="B77" s="7" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>176</v>
-      </c>
+      <c r="B77" s="7"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>173</v>
       </c>
       <c r="B78" s="7" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>177</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -5771,14 +5781,14 @@
         <v>173</v>
       </c>
       <c r="B79" s="7" t="str">
-        <f>"4"</f>
-        <v>4</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -5786,14 +5796,14 @@
         <v>173</v>
       </c>
       <c r="B80" s="7" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C80" s="23" t="s">
-        <v>180</v>
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -5801,14 +5811,14 @@
         <v>173</v>
       </c>
       <c r="B81" s="7" t="str">
-        <f>"6"</f>
-        <v>6</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>182</v>
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -5816,14 +5826,14 @@
         <v>173</v>
       </c>
       <c r="B82" s="7" t="str">
-        <f>"7"</f>
-        <v>7</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>243</v>
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>180</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -5831,14 +5841,14 @@
         <v>173</v>
       </c>
       <c r="B83" s="7" t="str">
-        <f>"8"</f>
-        <v>8</v>
+        <f>"6"</f>
+        <v>6</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -5846,14 +5856,14 @@
         <v>173</v>
       </c>
       <c r="B84" s="7" t="str">
-        <f>"9"</f>
-        <v>9</v>
-      </c>
-      <c r="C84" s="23" t="s">
-        <v>187</v>
+        <f>"7"</f>
+        <v>7</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -5861,14 +5871,14 @@
         <v>173</v>
       </c>
       <c r="B85" s="7" t="str">
-        <f>"11"</f>
-        <v>11</v>
+        <f>"8"</f>
+        <v>8</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>424</v>
+        <v>185</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>425</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -5876,14 +5886,14 @@
         <v>173</v>
       </c>
       <c r="B86" s="7" t="str">
-        <f>"12"</f>
-        <v>12</v>
+        <f>"9"</f>
+        <v>9</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>452</v>
+        <v>187</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>453</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -5891,63 +5901,63 @@
         <v>173</v>
       </c>
       <c r="B87" s="7" t="str">
+        <f>"11"</f>
+        <v>11</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="7" t="str">
+        <f>"12"</f>
+        <v>12</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>452</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>173</v>
+      </c>
+      <c r="B89" s="7" t="str">
         <f>"10"</f>
         <v>10</v>
       </c>
-      <c r="C87" s="23" t="s">
+      <c r="C89" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="7"/>
-      <c r="C88" s="23"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>191</v>
-      </c>
-      <c r="B89" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C89" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>191</v>
-      </c>
-      <c r="B90" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C90" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>195</v>
-      </c>
+      <c r="B90" s="7"/>
+      <c r="C90" s="23"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>191</v>
       </c>
       <c r="B91" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>454</v>
+        <v>193</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>455</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -5955,210 +5965,210 @@
         <v>191</v>
       </c>
       <c r="B92" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>191</v>
       </c>
-      <c r="B93" s="7" t="str">
+      <c r="B93" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C93" s="23" t="s">
+        <v>454</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="7" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C93" s="23" t="s">
+      <c r="C95" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="7"/>
-      <c r="C94" s="23"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="7"/>
+      <c r="C96" s="23"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>200</v>
       </c>
-      <c r="B95" t="str">
+      <c r="B97" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C95" s="23" t="s">
+      <c r="C97" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>200</v>
       </c>
-      <c r="B96" t="str">
+      <c r="B98" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C96" s="23" t="s">
+      <c r="C98" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="7"/>
-      <c r="C97" s="23"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>205</v>
-      </c>
-      <c r="B98" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C98" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>205</v>
-      </c>
-      <c r="B99" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C99" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>207</v>
-      </c>
+      <c r="B99" s="7"/>
+      <c r="C99" s="23"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>205</v>
       </c>
       <c r="B100" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C100" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>205</v>
+      </c>
+      <c r="B101" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C101" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>205</v>
+      </c>
+      <c r="B102" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C102" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="7"/>
-      <c r="C101" s="23"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>210</v>
-      </c>
-      <c r="B102" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C102" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>210</v>
-      </c>
-      <c r="B103" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C103" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="B103" s="7"/>
+      <c r="C103" s="23"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>210</v>
       </c>
       <c r="B104" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C104" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D106" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="7"/>
-      <c r="C105" s="23"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>214</v>
-      </c>
-      <c r="B106" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C106" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>214</v>
-      </c>
-      <c r="B107" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C107" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="B107" s="7"/>
+      <c r="C107" s="23"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>214</v>
       </c>
       <c r="B108" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>467</v>
+        <v>215</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>466</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -6166,111 +6176,111 @@
         <v>214</v>
       </c>
       <c r="B109" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C109" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>214</v>
+      </c>
+      <c r="B111" t="str">
         <f>"6"</f>
         <v>6</v>
       </c>
-      <c r="C109" s="23" t="s">
+      <c r="C111" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D111" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="23"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>479</v>
-      </c>
-      <c r="B111" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C111" s="23" t="s">
-        <v>480</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>483</v>
-      </c>
-    </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>479</v>
-      </c>
-      <c r="B112" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C112" s="23" t="s">
-        <v>481</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>484</v>
-      </c>
+      <c r="C112" s="23"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>479</v>
       </c>
       <c r="B113" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C113" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>479</v>
+      </c>
+      <c r="B114" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C114" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>479</v>
+      </c>
+      <c r="B115" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C113" s="23" t="s">
+      <c r="C115" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D115" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="7"/>
-      <c r="C114" s="23"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>218</v>
-      </c>
-      <c r="B115" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C115" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>218</v>
-      </c>
-      <c r="B116" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C116" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>221</v>
-      </c>
+      <c r="B116" s="7"/>
+      <c r="C116" s="23"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>218</v>
       </c>
       <c r="B117" t="str">
-        <f>"5"</f>
-        <v>5</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>463</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C117" s="23" t="s">
+        <v>232</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>465</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -6278,21 +6288,45 @@
         <v>218</v>
       </c>
       <c r="B118" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C118" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>218</v>
+      </c>
+      <c r="B119" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>218</v>
+      </c>
+      <c r="B120" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D120" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="7"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="7"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="7"/>
@@ -6338,6 +6372,12 @@
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="7"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="7"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>